<commit_message>
chg: Updated target list
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
+++ b/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18492" windowHeight="11700" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18492" windowHeight="11700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Target list" sheetId="1" r:id="rId1"/>
-    <sheet name="JPTL D+2" sheetId="3" r:id="rId2"/>
-    <sheet name="Example_support" sheetId="4" r:id="rId3"/>
+    <sheet name="JPTL D+X" sheetId="3" r:id="rId2"/>
+    <sheet name="JPTL D+X EXAMPLE" sheetId="5" r:id="rId3"/>
+    <sheet name="Explanation" sheetId="6" r:id="rId4"/>
+    <sheet name="Example_support" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="127">
   <si>
     <t>OP ACTIVE RESOLVE TARGET LIST</t>
   </si>
@@ -159,9 +161,6 @@
     <t>High Value Target</t>
   </si>
   <si>
-    <t>Current as of: G+0</t>
-  </si>
-  <si>
     <t>BDA</t>
   </si>
   <si>
@@ -171,12 +170,6 @@
     <t>Updated by:</t>
   </si>
   <si>
-    <t>JPTL with priority</t>
-  </si>
-  <si>
-    <t>TST matrix</t>
-  </si>
-  <si>
     <t>Source:</t>
   </si>
   <si>
@@ -192,14 +185,240 @@
     <t>JPUB Joint Targeting (Unclassified):</t>
   </si>
   <si>
-    <t xml:space="preserve">JPTL produced for each ATO </t>
+    <t>Current as of: D+0</t>
+  </si>
+  <si>
+    <t>PRIORITY</t>
+  </si>
+  <si>
+    <t>OBJECTIVE NAME</t>
+  </si>
+  <si>
+    <t>TARGET</t>
+  </si>
+  <si>
+    <t>D+X</t>
+  </si>
+  <si>
+    <t>ELEVATION</t>
+  </si>
+  <si>
+    <t>DESIRED EFFECT</t>
+  </si>
+  <si>
+    <t>TARGET NUMBER</t>
+  </si>
+  <si>
+    <t>TARGET CATEGORY</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>RISK LEVEL</t>
+  </si>
+  <si>
+    <t>ATO DAY:</t>
+  </si>
+  <si>
+    <t>TST targets are to be struck immediatly when detected. These are high priority targets for the entire force.</t>
+  </si>
+  <si>
+    <t>JPTL produced for each ATO . These targets are to be planned to be attacked during the ATO day</t>
+  </si>
+  <si>
+    <t>D+12</t>
+  </si>
+  <si>
+    <t>VIS (NECK)</t>
+  </si>
+  <si>
+    <t>UNLOCATED</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>DESTROY</t>
+  </si>
+  <si>
+    <t>OPARTGT201</t>
+  </si>
+  <si>
+    <t>DOLLY</t>
+  </si>
+  <si>
+    <t>N23 23.333</t>
+  </si>
+  <si>
+    <t>E053 34.567</t>
+  </si>
+  <si>
+    <t>345ft</t>
+  </si>
+  <si>
+    <t>DENY USE OF RWY FOR 24 HOURS</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>OPARTGT211</t>
+  </si>
+  <si>
+    <t>MINNY</t>
+  </si>
+  <si>
+    <t>CORPS HQ</t>
+  </si>
+  <si>
+    <t>N21.12.345</t>
+  </si>
+  <si>
+    <t>E023 12.345</t>
+  </si>
+  <si>
+    <t>1244ft</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>OPARTGT109</t>
+  </si>
+  <si>
+    <t>SCROOGE</t>
+  </si>
+  <si>
+    <t>AIRFIELD 1</t>
+  </si>
+  <si>
+    <t>For targets to be put on JPTL they need minimum to be fixed in time and space</t>
+  </si>
+  <si>
+    <t>TST targets are not fixed in time and space</t>
+  </si>
+  <si>
+    <t>AWACS</t>
+  </si>
+  <si>
+    <t>20000ft</t>
+  </si>
+  <si>
+    <t>SILKWORM MISSILES</t>
+  </si>
+  <si>
+    <t>UNKNOWN, INTELIGENCE REPORTS SIGHTING WEST OF VILLAGE 1</t>
+  </si>
+  <si>
+    <t>N20 11.111</t>
+  </si>
+  <si>
+    <t>E011 11.111</t>
+  </si>
+  <si>
+    <t>KILL</t>
+  </si>
+  <si>
+    <t>EXTREME</t>
+  </si>
+  <si>
+    <t>CHEMICAL WEAPON LOADED SCUD</t>
+  </si>
+  <si>
+    <t>LAST REPORTED IN VILLAGE 2</t>
+  </si>
+  <si>
+    <t>One BN of the 923rd SSM Regiment is loaded with chemical weapons</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JOINT PRIORITIZED TARGET LIST (JPTL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TIME SENSITIVE TARGET MATRIX (TST)</t>
+  </si>
+  <si>
+    <t>OPERATION ACTIVE RESOLVE</t>
+  </si>
+  <si>
+    <t>DEFINITION</t>
+  </si>
+  <si>
+    <t>CLARIFICATION</t>
+  </si>
+  <si>
+    <t>Losses only at expected training or peactime attrition rates</t>
+  </si>
+  <si>
+    <t>losses expected at historical combat rates. Accept neutral or disadvantegous engagements can withdraw to prevent heavy losses</t>
+  </si>
+  <si>
+    <t>Accept losses to achieve objective. Preserve future capability if able</t>
+  </si>
+  <si>
+    <t>Losses may result in complete force annihilation. Accept any losses necessary to accomplish mission</t>
+  </si>
+  <si>
+    <t>Force survival high priority</t>
+  </si>
+  <si>
+    <t>Whenever possible, provide SEAD support to operations in known SAM envelopes and position recovery forces at FOBs</t>
+  </si>
+  <si>
+    <t>Operations in known SAM envelopes without SEAD support. PR missions and recovery forces at FOL/FARP</t>
+  </si>
+  <si>
+    <t>Defense against WMD, where consequences of failure unaceptable.</t>
+  </si>
+  <si>
+    <t>ACCEPTED RISK LEVELS</t>
+  </si>
+  <si>
+    <t>TARGET CATEGORIES</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Targets absolutely must be tasked for attack on this ATO because:
+- The target is essential for mission success in support of current objectives (or is a designated HPT, High Payoff Target, or TST
+- It is crucial to the overall success of the operation
+- It will have immediate and compelling effects
+- Its timeliness as an urgent target may not exist in the future
+- If not targeted, negative consequences may seriously jeopardize future CJTF operations</t>
+  </si>
+  <si>
+    <t>CRITERIA</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>Targets desired to be tasked for attack on this ATO because:
+- It will contribute to the battle, but it is not critical to mission success
+- It will further the success of the operation
+- It will eventually require targetding due to JFC future plans
+- If not targeted on this ATO, negative consequences will probably not impede operations</t>
+  </si>
+  <si>
+    <t>Targets need to be tasked for attack on this ATO because:
+- Targets have substantial, but not immediate impact on the battle
+- The cascading effects this target provides may not be realized in the future
+- If not targeted on this ATO, a significant level of effort may be required later
+- If not targeted , negative consequence smay significantly hamper CJTF operations</t>
+  </si>
+  <si>
+    <t>Target folders may be produced (Should?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,8 +459,56 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +527,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -338,30 +617,182 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -370,7 +801,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -381,7 +823,96 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -393,22 +924,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -423,130 +939,9 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -560,9 +955,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,54 +971,202 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
@@ -634,16 +1181,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -661,7 +1208,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8717280" y="1097280"/>
+          <a:off x="13220700" y="0"/>
           <a:ext cx="4175760" cy="2712720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -681,16 +1228,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -708,7 +1255,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6080760" y="2438400"/>
+          <a:off x="8016240" y="350520"/>
           <a:ext cx="4975860" cy="6156960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -728,16 +1275,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -755,7 +1302,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11094720" y="4937760"/>
+          <a:off x="11285220" y="6103620"/>
           <a:ext cx="5128260" cy="2567940"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -822,16 +1369,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>670560</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -849,7 +1396,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5349240" y="1295400"/>
+          <a:off x="861060" y="1310640"/>
           <a:ext cx="5166360" cy="2415540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -869,16 +1416,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>967740</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -896,7 +1443,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="1424940"/>
+          <a:off x="1760220" y="1600200"/>
           <a:ext cx="5806440" cy="6743700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1202,492 +1749,548 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I317"/>
+  <dimension ref="A1:J317"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.21875" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="28.77734375" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21.6" thickBot="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" ht="21.6" thickBot="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="29.4" customHeight="1" thickBot="1">
+      <c r="A3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="21"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="15" t="s">
+      <c r="J3" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="23" t="s">
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="17"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="23" t="s">
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="23" t="s">
+      <c r="I5" s="13"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="23" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="23" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="23" t="s">
+      <c r="H8" s="11"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
+      <c r="D9" s="12"/>
+      <c r="E9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="17"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="23" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="17"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="23" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="23" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="17"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="23" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="17"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="23" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="17"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="23" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="23" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="17"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="23" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="23" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="17"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="23" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="17"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="23" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="17"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="23" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="23" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="17"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="23" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="17"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="23" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="17"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="23" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="17"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="23" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="23" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="23" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="23" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="17"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="23" t="s">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="17"/>
-    </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1">
-      <c r="A31" s="24" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" thickBot="1">
+      <c r="A31" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="18"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4549,118 +5152,1082 @@
     </row>
   </sheetData>
   <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21">
+      <c r="A1" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="59"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1">
+      <c r="A2" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="67"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1">
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6">
+      <c r="A4" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="69" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="35">
+        <v>1</v>
+      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="37"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="35">
+        <v>2</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="37"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="35">
+        <v>3</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="35">
+        <v>4</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="37"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="35">
+        <v>5</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="35">
+        <v>6</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="35">
+        <v>7</v>
+      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="37"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" thickBot="1">
+      <c r="A13" s="38">
+        <v>8</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.6">
+      <c r="A15" s="73" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="75"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="30"/>
+      <c r="I16" s="34"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="32">
+        <v>1</v>
+      </c>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="K17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="32">
+        <v>2</v>
+      </c>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="32">
+        <v>3</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="32">
+        <v>4</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="32">
+        <v>5</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="32">
+        <v>6</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="32">
+        <v>7</v>
+      </c>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="45"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="32">
+        <v>8</v>
+      </c>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="32">
+        <v>9</v>
+      </c>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1">
+      <c r="A26" s="33">
+        <v>10</v>
+      </c>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="28"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-      <c r="K3" t="s">
+    <row r="1" spans="1:17" ht="21">
+      <c r="A1" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="59"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" thickBot="1">
+      <c r="A2" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="67"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" thickBot="1"/>
+    <row r="4" spans="1:17" ht="15.6">
+      <c r="A4" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="56" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" thickBot="1"/>
-    <row r="6" spans="1:11">
-      <c r="A6" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="29"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="34"/>
+      <c r="E5" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="31.8">
+      <c r="A6" s="35">
+        <v>1</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55"/>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="35">
+        <v>2</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="55"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="35">
+        <v>3</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="35">
+        <v>4</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="37"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="35">
+        <v>5</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="35">
+        <v>6</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="35">
+        <v>7</v>
+      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="37"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" thickBot="1">
+      <c r="A13" s="38">
+        <v>8</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" thickBot="1">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" ht="15.6">
+      <c r="A15" s="73" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="75"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="30"/>
+      <c r="I16" s="34"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="32">
+        <v>1</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="43"/>
+      <c r="G17" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+    </row>
+    <row r="18" spans="1:11" ht="28.8">
+      <c r="A18" s="32">
+        <v>2</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="43"/>
+      <c r="G18" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+    </row>
+    <row r="19" spans="1:11" ht="43.2">
+      <c r="A19" s="32">
+        <v>3</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="43"/>
+      <c r="G19" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
+      <c r="K19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="32">
+        <v>4</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="32">
+        <v>5</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+      <c r="K21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="32">
+        <v>6</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="32">
+        <v>7</v>
+      </c>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="45"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="32">
+        <v>8</v>
+      </c>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="32">
+        <v>9</v>
+      </c>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1">
+      <c r="A26" s="33">
+        <v>10</v>
+      </c>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
     </row>
   </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A5:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="46.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:3">
+      <c r="A5" s="77" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="78" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="78" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8">
+      <c r="A7" s="80" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57.6">
+      <c r="A8" s="80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="79" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.8">
+      <c r="A9" s="80" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="79" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="43.2">
+      <c r="A10" s="80" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="79" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="82" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="77"/>
+    </row>
+    <row r="15" spans="1:3" ht="109.8" customHeight="1">
+      <c r="A15" s="80" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="81"/>
+    </row>
+    <row r="16" spans="1:3" ht="79.2" customHeight="1">
+      <c r="A16" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="81"/>
+    </row>
+    <row r="17" spans="1:3" ht="87" customHeight="1">
+      <c r="A17" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="81" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="81"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C5"/>
   <sheetViews>
@@ -4675,24 +6242,24 @@
   <sheetData>
     <row r="2" spans="2:3">
       <c r="B2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="7.2" customHeight="1"/>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chg: Added CJTF-82 logo to the Target list
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
+++ b/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18492" windowHeight="11700" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18492" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Target list" sheetId="1" r:id="rId1"/>
@@ -435,13 +435,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -507,6 +500,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -540,7 +540,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -947,10 +947,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -961,82 +998,61 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1048,20 +1064,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1087,28 +1111,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1118,54 +1135,74 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1178,6 +1215,138 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>111125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7432</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>682625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>611188</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect l="10867" t="8733" r="9569" b="8792"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8231188" y="7432"/>
+          <a:ext cx="571500" cy="603756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>611376</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect l="10867" t="8733" r="9569" b="8792"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6766560" y="7620"/>
+          <a:ext cx="571500" cy="603756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>618996</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect l="10867" t="8733" r="9569" b="8792"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6774180" y="15240"/>
+          <a:ext cx="571500" cy="603756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1751,8 +1920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J317"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1768,19 +1937,19 @@
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21.6" thickBot="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" ht="49.95" customHeight="1" thickBot="1">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1799,496 +1968,496 @@
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="29.4" customHeight="1" thickBot="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="24"/>
-      <c r="J4" s="25"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="14"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="14"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="14"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="14"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="14"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="14"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="14"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="14"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="14"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="14"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="14"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="14"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="14"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="14"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1"/>
@@ -5156,6 +5325,7 @@
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5164,7 +5334,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -5179,35 +5349,35 @@
     <col min="9" max="9" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:11" ht="49.95" customHeight="1">
+      <c r="A1" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="59"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="82"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="62" t="s">
+      <c r="B2" s="72"/>
+      <c r="C2" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="67"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1">
       <c r="K3" t="s">
@@ -5215,150 +5385,150 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.6">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="72"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="H5" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="69" t="s">
+      <c r="I5" s="39" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="35">
+      <c r="A6" s="28">
         <v>1</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="35">
+      <c r="A7" s="28">
         <v>2</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="37"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="35">
+      <c r="A8" s="28">
         <v>3</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="35">
+      <c r="A9" s="28">
         <v>4</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="35">
+      <c r="A10" s="28">
         <v>5</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="35">
+      <c r="A11" s="28">
         <v>6</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="35">
+      <c r="A12" s="28">
         <v>7</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1">
-      <c r="A13" s="38">
+      <c r="A13" s="31">
         <v>8</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1">
       <c r="A14" s="1"/>
@@ -5372,183 +5542,181 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15.6">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="75"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="28" t="s">
+      <c r="F16" s="70"/>
+      <c r="G16" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="34"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="69"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="32">
+      <c r="A17" s="26">
         <v>1</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
       <c r="K17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="32">
+      <c r="A18" s="26">
         <v>2</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="45"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="32">
+      <c r="A19" s="26">
         <v>3</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="45"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="54"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="32">
+      <c r="A20" s="26">
         <v>4</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="32">
+      <c r="A21" s="26">
         <v>5</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="32">
+      <c r="A22" s="26">
         <v>6</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="54"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="32">
+      <c r="A23" s="26">
         <v>7</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="32">
+      <c r="A24" s="26">
         <v>8</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="32">
+      <c r="A25" s="26">
         <v>9</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
-      <c r="A26" s="33">
+      <c r="A26" s="27">
         <v>10</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="54"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="D2:G2"/>
@@ -5565,14 +5733,17 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5580,8 +5751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -5596,78 +5767,78 @@
     <col min="9" max="9" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:17" ht="49.95" customHeight="1">
+      <c r="A1" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="59"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="82"/>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="62" t="s">
+      <c r="B2" s="72"/>
+      <c r="C2" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66" t="s">
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="67"/>
+      <c r="I2" s="56"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.6">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="72"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="H5" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="69" t="s">
+      <c r="I5" s="39" t="s">
         <v>66</v>
       </c>
       <c r="K5" t="s">
@@ -5675,174 +5846,174 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="31.8">
-      <c r="A6" s="35">
+      <c r="A6" s="28">
         <v>1</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="I6" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="55" t="s">
+      <c r="K6" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="55"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="35">
+      <c r="A7" s="28">
         <v>2</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="I7" s="37" t="s">
+      <c r="I7" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="55" t="s">
+      <c r="K7" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="55"/>
-      <c r="Q7" s="55"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="35">
+      <c r="A8" s="28">
         <v>3</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="35">
+      <c r="A9" s="28">
         <v>4</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="35">
+      <c r="A10" s="28">
         <v>5</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="35">
+      <c r="A11" s="28">
         <v>6</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="35">
+      <c r="A12" s="28">
         <v>7</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:17" ht="15" thickBot="1">
-      <c r="A13" s="38">
+      <c r="A13" s="31">
         <v>8</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:17" ht="15" thickBot="1">
       <c r="A14" s="1"/>
@@ -5856,209 +6027,223 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="15.6">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="75"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="28" t="s">
+      <c r="F16" s="70"/>
+      <c r="G16" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="34"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="69"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="32">
+      <c r="A17" s="26">
         <v>1</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="42" t="s">
+      <c r="F17" s="66"/>
+      <c r="G17" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
     </row>
     <row r="18" spans="1:11" ht="28.8">
-      <c r="A18" s="32">
+      <c r="A18" s="26">
         <v>2</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="42" t="s">
+      <c r="F18" s="66"/>
+      <c r="G18" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="44"/>
-      <c r="I18" s="45"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
     </row>
     <row r="19" spans="1:11" ht="43.2">
-      <c r="A19" s="32">
+      <c r="A19" s="26">
         <v>3</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="41" t="s">
+      <c r="D19" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="42" t="s">
+      <c r="F19" s="66"/>
+      <c r="G19" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="H19" s="44"/>
-      <c r="I19" s="45"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="54"/>
       <c r="K19" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="32">
+      <c r="A20" s="26">
         <v>4</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="32">
+      <c r="A21" s="26">
         <v>5</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="54"/>
       <c r="K21" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="32">
+      <c r="A22" s="26">
         <v>6</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="54"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="32">
+      <c r="A23" s="26">
         <v>7</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="32">
+      <c r="A24" s="26">
         <v>8</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="32">
+      <c r="A25" s="26">
         <v>9</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
-      <c r="A26" s="33">
+      <c r="A26" s="27">
         <v>10</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="54"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="K6:Q6"/>
@@ -6075,23 +6260,10 @@
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:I20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6099,8 +6271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -6110,118 +6282,118 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:3">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="41" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="42" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="57.6">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="42" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="42" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="43.2">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="42" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="77"/>
+      <c r="C14" s="74"/>
     </row>
     <row r="15" spans="1:3" ht="109.8" customHeight="1">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="81"/>
+      <c r="C15" s="75"/>
     </row>
     <row r="16" spans="1:3" ht="79.2" customHeight="1">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="81"/>
+      <c r="C16" s="75"/>
     </row>
     <row r="17" spans="1:3" ht="87" customHeight="1">
-      <c r="A17" s="80" t="s">
+      <c r="A17" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="81"/>
+      <c r="C17" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chg: Added VIS and JFACC instruction file. Added logo to target file. Added objectives to CJTF 82 OPORDER
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
+++ b/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
@@ -992,7 +992,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1087,6 +1087,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1120,89 +1129,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1218,16 +1230,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>111125</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>87313</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>7432</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>682625</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>658813</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>611188</xdr:rowOff>
+      <xdr:rowOff>603756</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1245,8 +1257,47 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8231188" y="7432"/>
+          <a:off x="87313" y="0"/>
           <a:ext cx="571500" cy="603756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>771867</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>580031</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect l="5045" t="7763" r="8763" b="8014"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8310563" y="0"/>
+          <a:ext cx="581367" cy="580031"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1262,14 +1313,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>611376</xdr:rowOff>
     </xdr:to>
@@ -1289,8 +1340,47 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6766560" y="7620"/>
+          <a:off x="30480" y="7620"/>
           <a:ext cx="571500" cy="603756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>649947</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>602891</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect l="5045" t="7763" r="8763" b="8014"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6789420" y="22860"/>
+          <a:ext cx="581367" cy="580031"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1306,16 +1396,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>618996</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1776</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1333,8 +1423,47 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6774180" y="15240"/>
+          <a:off x="99060" y="30480"/>
           <a:ext cx="571500" cy="603756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28233</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>595271</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect l="5045" t="7763" r="8763" b="8014"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6749073" y="15240"/>
+          <a:ext cx="581367" cy="580031"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1921,7 +2050,7 @@
   <dimension ref="A1:J317"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1938,18 +2067,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="49.95" customHeight="1" thickBot="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -5334,7 +5463,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -5350,34 +5479,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.95" customHeight="1">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="82"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="74"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="72"/>
+      <c r="B2" s="76"/>
       <c r="C2" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="56"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="78"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1">
       <c r="K3" t="s">
@@ -5385,17 +5514,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.6">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="62"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="38" t="s">
@@ -5542,17 +5671,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15.6">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="65"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="66"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="25" t="s">
@@ -5567,15 +5696,15 @@
       <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="70"/>
-      <c r="G16" s="67" t="s">
+      <c r="F16" s="71"/>
+      <c r="G16" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="68"/>
-      <c r="I16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="70"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="26">
@@ -5584,11 +5713,11 @@
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="54"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="57"/>
       <c r="K17" t="s">
         <v>68</v>
       </c>
@@ -5600,11 +5729,11 @@
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="54"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="57"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="26">
@@ -5613,11 +5742,11 @@
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="54"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="57"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="26">
@@ -5626,11 +5755,11 @@
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="54"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="57"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="26">
@@ -5639,11 +5768,11 @@
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="54"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="57"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="26">
@@ -5652,11 +5781,11 @@
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="54"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="26">
@@ -5665,11 +5794,11 @@
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="54"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="57"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="26">
@@ -5678,11 +5807,11 @@
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="54"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="57"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="26">
@@ -5691,11 +5820,11 @@
       <c r="B25" s="35"/>
       <c r="C25" s="35"/>
       <c r="D25" s="35"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="27">
@@ -5704,27 +5833,22 @@
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
       <c r="D26" s="32"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="G24:I24"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="G18:I18"/>
@@ -5733,6 +5857,9 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E26:F26"/>
@@ -5740,6 +5867,8 @@
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5752,7 +5881,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -5768,50 +5897,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.95" customHeight="1">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="82"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="74"/>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="72"/>
+      <c r="B2" s="76"/>
       <c r="C2" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="55" t="s">
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="56"/>
+      <c r="I2" s="78"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.6">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="62"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="38" t="s">
@@ -5873,15 +6002,15 @@
       <c r="I6" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="73" t="s">
+      <c r="K6" s="79" t="s">
         <v>92</v>
       </c>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="28">
@@ -5911,15 +6040,15 @@
       <c r="I7" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="73" t="s">
+      <c r="K7" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="79"/>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="79"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="28">
@@ -6027,17 +6156,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="15.6">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="65"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="66"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="25" t="s">
@@ -6052,84 +6181,84 @@
       <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="70"/>
-      <c r="G16" s="67" t="s">
+      <c r="F16" s="71"/>
+      <c r="G16" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="68"/>
-      <c r="I16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="70"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="26">
         <v>1</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="66"/>
-      <c r="G17" s="52" t="s">
+      <c r="F17" s="81"/>
+      <c r="G17" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="53"/>
-      <c r="I17" s="54"/>
-    </row>
-    <row r="18" spans="1:11" ht="28.8">
+      <c r="H17" s="82"/>
+      <c r="I17" s="83"/>
+    </row>
+    <row r="18" spans="1:11" ht="21.6">
       <c r="A18" s="26">
         <v>2</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="66"/>
-      <c r="G18" s="52" t="s">
+      <c r="F18" s="81"/>
+      <c r="G18" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="53"/>
-      <c r="I18" s="54"/>
-    </row>
-    <row r="19" spans="1:11" ht="43.2">
+      <c r="H18" s="82"/>
+      <c r="I18" s="83"/>
+    </row>
+    <row r="19" spans="1:11" ht="31.8">
       <c r="A19" s="26">
         <v>3</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="66"/>
-      <c r="G19" s="52" t="s">
+      <c r="F19" s="81"/>
+      <c r="G19" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="H19" s="53"/>
-      <c r="I19" s="54"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="83"/>
       <c r="K19" t="s">
         <v>68</v>
       </c>
@@ -6141,11 +6270,11 @@
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="54"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="57"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="26">
@@ -6154,11 +6283,11 @@
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="54"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="57"/>
       <c r="K21" t="s">
         <v>93</v>
       </c>
@@ -6170,11 +6299,11 @@
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="54"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="26">
@@ -6183,11 +6312,11 @@
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="54"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="57"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="26">
@@ -6196,11 +6325,11 @@
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="54"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="57"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="26">
@@ -6209,11 +6338,11 @@
       <c r="B25" s="35"/>
       <c r="C25" s="35"/>
       <c r="D25" s="35"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="27">
@@ -6222,11 +6351,11 @@
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
       <c r="D26" s="32"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -6282,11 +6411,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:3">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="41" t="s">
@@ -6344,47 +6473,47 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="74"/>
+      <c r="C14" s="85"/>
     </row>
     <row r="15" spans="1:3" ht="109.8" customHeight="1">
       <c r="A15" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="84" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="75"/>
+      <c r="C15" s="84"/>
     </row>
     <row r="16" spans="1:3" ht="79.2" customHeight="1">
       <c r="A16" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="84" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="75"/>
+      <c r="C16" s="84"/>
     </row>
     <row r="17" spans="1:3" ht="87" customHeight="1">
       <c r="A17" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="75"/>
+      <c r="C17" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
chg: Update to various documents
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
+++ b/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18492" windowHeight="11700"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Target list" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Explanation" sheetId="6" r:id="rId4"/>
     <sheet name="Example_support" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="131">
   <si>
     <t>OP ACTIVE RESOLVE TARGET LIST</t>
   </si>
@@ -412,6 +412,21 @@
   </si>
   <si>
     <t>Target folders may be produced (Should?)</t>
+  </si>
+  <si>
+    <t>EXPLANATION</t>
+  </si>
+  <si>
+    <t>EXPLANATION /SIGNIFICANCE</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Target of oppertunity if other targets not suitable for this ATO
+- It will have minor contributions to the operation
+- It may be required for targeting, but is not time critical
+- If not targeted, no negative consequences</t>
   </si>
 </sst>
 </file>
@@ -508,7 +523,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -539,8 +554,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -982,6 +1003,74 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -992,7 +1081,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1012,13 +1101,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1087,6 +1169,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1129,23 +1245,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1155,9 +1256,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1190,6 +1288,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1272,13 +1388,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19844</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>771867</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>580031</xdr:rowOff>
+      <xdr:rowOff>599875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1296,7 +1412,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8310563" y="0"/>
+          <a:off x="8128000" y="19844"/>
           <a:ext cx="581367" cy="580031"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1479,6 +1595,58 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>695325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8191500" y="3095625"/>
+          <a:ext cx="6877050" cy="3181350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>617220</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -1498,7 +1666,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1545,7 +1713,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1592,7 +1760,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1639,7 +1807,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1686,7 +1854,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1733,7 +1901,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1743,6 +1911,53 @@
         <a:xfrm>
           <a:off x="1760220" y="1600200"/>
           <a:ext cx="5806440" cy="6743700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6800850" y="4286250"/>
+          <a:ext cx="7600950" cy="5334000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2047,40 +2262,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J317"/>
+  <dimension ref="A1:N317"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="78.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49.95" customHeight="1" thickBot="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:14" ht="49.9" customHeight="1" thickBot="1">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
-    </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="67"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -2095,68 +2320,97 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="29.4" customHeight="1" thickBot="1">
-      <c r="A3" s="23" t="s">
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
+    </row>
+    <row r="3" spans="1:14" ht="29.45" customHeight="1" thickBot="1">
+      <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="18" t="s">
+      <c r="K3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="62" t="str">
+        <f>A4</f>
+        <v>OPARTGT001</v>
+      </c>
+      <c r="L4" s="63" t="str">
+        <f>B4</f>
+        <v>922nd SSM Regiment</v>
+      </c>
+      <c r="M4" s="63" t="str">
+        <f>C4</f>
+        <v>SCUDs</v>
+      </c>
+      <c r="N4" s="43"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -2183,8 +2437,21 @@
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="62" t="str">
+        <f t="shared" ref="K5:K29" si="0">A5</f>
+        <v>OPARTGT002</v>
+      </c>
+      <c r="L5" s="63" t="str">
+        <f t="shared" ref="L5:L29" si="1">B5</f>
+        <v>923rd SSM Regiment</v>
+      </c>
+      <c r="M5" s="63" t="str">
+        <f t="shared" ref="M5:M29" si="2">C5</f>
+        <v>SCUDs</v>
+      </c>
+      <c r="N5" s="44"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -2207,8 +2474,21 @@
       <c r="H6" s="8"/>
       <c r="I6" s="10"/>
       <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT003</v>
+      </c>
+      <c r="L6" s="63" t="str">
+        <f t="shared" si="1"/>
+        <v>141st Heavy Rocket Artillery BN</v>
+      </c>
+      <c r="M6" s="63" t="str">
+        <f t="shared" si="2"/>
+        <v>MLRS</v>
+      </c>
+      <c r="N6" s="44"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -2231,8 +2511,21 @@
       <c r="H7" s="8"/>
       <c r="I7" s="10"/>
       <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT004</v>
+      </c>
+      <c r="L7" s="63" t="str">
+        <f t="shared" si="1"/>
+        <v>142nd Heavy Rocket Artillery BN</v>
+      </c>
+      <c r="M7" s="63" t="str">
+        <f t="shared" si="2"/>
+        <v>MLRS</v>
+      </c>
+      <c r="N7" s="44"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2255,8 +2548,21 @@
       <c r="H8" s="8"/>
       <c r="I8" s="10"/>
       <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT005</v>
+      </c>
+      <c r="L8" s="63" t="str">
+        <f t="shared" si="1"/>
+        <v>341st Heavy Rocket Artillery BN</v>
+      </c>
+      <c r="M8" s="63" t="str">
+        <f t="shared" si="2"/>
+        <v>MLRS</v>
+      </c>
+      <c r="N8" s="44"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
@@ -2279,8 +2585,21 @@
       <c r="H9" s="8"/>
       <c r="I9" s="10"/>
       <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT006</v>
+      </c>
+      <c r="L9" s="63" t="str">
+        <f t="shared" si="1"/>
+        <v>342nd Heavy Rocket Artillery BN</v>
+      </c>
+      <c r="M9" s="63" t="str">
+        <f t="shared" si="2"/>
+        <v>MLRS</v>
+      </c>
+      <c r="N9" s="44"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
@@ -2293,8 +2612,21 @@
       <c r="H10" s="8"/>
       <c r="I10" s="10"/>
       <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT007</v>
+      </c>
+      <c r="L10" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="44"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -2307,8 +2639,21 @@
       <c r="H11" s="8"/>
       <c r="I11" s="10"/>
       <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT008</v>
+      </c>
+      <c r="L11" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="44"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
@@ -2321,8 +2666,21 @@
       <c r="H12" s="8"/>
       <c r="I12" s="10"/>
       <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT009</v>
+      </c>
+      <c r="L12" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="44"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
@@ -2335,8 +2693,21 @@
       <c r="H13" s="8"/>
       <c r="I13" s="10"/>
       <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT010</v>
+      </c>
+      <c r="L13" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="44"/>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
@@ -2349,8 +2720,21 @@
       <c r="H14" s="8"/>
       <c r="I14" s="10"/>
       <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT011</v>
+      </c>
+      <c r="L14" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="44"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="7" t="s">
         <v>24</v>
       </c>
@@ -2363,8 +2747,21 @@
       <c r="H15" s="8"/>
       <c r="I15" s="10"/>
       <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT012</v>
+      </c>
+      <c r="L15" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="44"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="7" t="s">
         <v>25</v>
       </c>
@@ -2377,8 +2774,21 @@
       <c r="H16" s="8"/>
       <c r="I16" s="10"/>
       <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT013</v>
+      </c>
+      <c r="L16" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="44"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
@@ -2391,8 +2801,21 @@
       <c r="H17" s="8"/>
       <c r="I17" s="10"/>
       <c r="J17" s="11"/>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT014</v>
+      </c>
+      <c r="L17" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="44"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="7" t="s">
         <v>27</v>
       </c>
@@ -2405,8 +2828,21 @@
       <c r="H18" s="8"/>
       <c r="I18" s="10"/>
       <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT015</v>
+      </c>
+      <c r="L18" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="44"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
@@ -2419,8 +2855,21 @@
       <c r="H19" s="8"/>
       <c r="I19" s="10"/>
       <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT016</v>
+      </c>
+      <c r="L19" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="44"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
@@ -2433,8 +2882,21 @@
       <c r="H20" s="8"/>
       <c r="I20" s="10"/>
       <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT017</v>
+      </c>
+      <c r="L20" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="44"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="7" t="s">
         <v>30</v>
       </c>
@@ -2447,8 +2909,21 @@
       <c r="H21" s="8"/>
       <c r="I21" s="10"/>
       <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT018</v>
+      </c>
+      <c r="L21" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="44"/>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="7" t="s">
         <v>31</v>
       </c>
@@ -2461,8 +2936,21 @@
       <c r="H22" s="8"/>
       <c r="I22" s="10"/>
       <c r="J22" s="11"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT019</v>
+      </c>
+      <c r="L22" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="44"/>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="7" t="s">
         <v>32</v>
       </c>
@@ -2475,8 +2963,21 @@
       <c r="H23" s="8"/>
       <c r="I23" s="10"/>
       <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT020</v>
+      </c>
+      <c r="L23" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="44"/>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="7" t="s">
         <v>33</v>
       </c>
@@ -2489,8 +2990,21 @@
       <c r="H24" s="8"/>
       <c r="I24" s="10"/>
       <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT021</v>
+      </c>
+      <c r="L24" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="44"/>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="7" t="s">
         <v>34</v>
       </c>
@@ -2503,8 +3017,21 @@
       <c r="H25" s="8"/>
       <c r="I25" s="10"/>
       <c r="J25" s="11"/>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT022</v>
+      </c>
+      <c r="L25" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="44"/>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="7" t="s">
         <v>35</v>
       </c>
@@ -2517,8 +3044,21 @@
       <c r="H26" s="8"/>
       <c r="I26" s="10"/>
       <c r="J26" s="11"/>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT023</v>
+      </c>
+      <c r="L26" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="44"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
@@ -2531,8 +3071,21 @@
       <c r="H27" s="8"/>
       <c r="I27" s="10"/>
       <c r="J27" s="11"/>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT024</v>
+      </c>
+      <c r="L27" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="44"/>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="7" t="s">
         <v>37</v>
       </c>
@@ -2545,360 +3098,580 @@
       <c r="H28" s="8"/>
       <c r="I28" s="10"/>
       <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="7" t="s">
+      <c r="K28" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT025</v>
+      </c>
+      <c r="L28" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="44"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A29" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="11"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="7" t="s">
+      <c r="B29" s="48"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>OPARTGT026</v>
+      </c>
+      <c r="L29" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="52"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="31" spans="1:10" ht="15" thickBot="1">
-      <c r="A31" s="13" t="s">
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="58"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="17"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="44"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="59"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="44"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="59"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="44"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="59"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="44"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="59"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="44"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="59"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="44"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="59"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="44"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="59"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="44"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="59"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="44"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="59"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="39"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="44"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="59"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="39"/>
+      <c r="M41" s="39"/>
+      <c r="N41" s="44"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="59"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="39"/>
+      <c r="M42" s="39"/>
+      <c r="N42" s="44"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="59"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="39"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="44"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="59"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="44"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="59"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="39"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="44"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="59"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="44"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="59"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="44"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="59"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="44"/>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="59"/>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="44"/>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="59"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="39"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="44"/>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="59"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="39"/>
+      <c r="J51" s="39"/>
+      <c r="K51" s="39"/>
+      <c r="L51" s="39"/>
+      <c r="M51" s="39"/>
+      <c r="N51" s="44"/>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="59"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="39"/>
+      <c r="L52" s="39"/>
+      <c r="M52" s="39"/>
+      <c r="N52" s="44"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="59"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="39"/>
+      <c r="J53" s="39"/>
+      <c r="K53" s="39"/>
+      <c r="L53" s="39"/>
+      <c r="M53" s="39"/>
+      <c r="N53" s="44"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="59"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="39"/>
+      <c r="L54" s="39"/>
+      <c r="M54" s="39"/>
+      <c r="N54" s="44"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="59"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="39"/>
+      <c r="L55" s="39"/>
+      <c r="M55" s="39"/>
+      <c r="N55" s="44"/>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="59"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="39"/>
+      <c r="L56" s="39"/>
+      <c r="M56" s="39"/>
+      <c r="N56" s="44"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="59"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="39"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="39"/>
+      <c r="L57" s="39"/>
+      <c r="M57" s="39"/>
+      <c r="N57" s="44"/>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="59"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="39"/>
+      <c r="L58" s="39"/>
+      <c r="M58" s="39"/>
+      <c r="N58" s="44"/>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="59"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="39"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="39"/>
+      <c r="L59" s="39"/>
+      <c r="M59" s="39"/>
+      <c r="N59" s="44"/>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="59"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="53"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="39"/>
+      <c r="N60" s="44"/>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="59"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="39"/>
+      <c r="J61" s="39"/>
+      <c r="K61" s="39"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="39"/>
+      <c r="N61" s="44"/>
+    </row>
+    <row r="62" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A62" s="60"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="61"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="45"/>
+      <c r="L62" s="45"/>
+      <c r="M62" s="45"/>
+      <c r="N62" s="46"/>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2908,7 +3681,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:14">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -5449,8 +6222,9 @@
       <c r="H317" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -5466,200 +6240,200 @@
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="49.95" customHeight="1">
-      <c r="A1" s="72" t="s">
+    <row r="1" spans="1:11" ht="49.9" customHeight="1">
+      <c r="A1" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="74"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1">
-      <c r="A2" s="75" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="89"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A2" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="91"/>
+      <c r="C2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="78"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="93"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="K3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6">
-      <c r="A4" s="61" t="s">
+    <row r="4" spans="1:11" ht="15.75">
+      <c r="A4" s="97" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="63"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="99"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="39" t="s">
+      <c r="I5" s="34" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="28">
+      <c r="A6" s="23">
         <v>1</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="28">
+      <c r="A7" s="23">
         <v>2</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="30"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="28">
+      <c r="A8" s="23">
         <v>3</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="30"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="28">
+      <c r="A9" s="23">
         <v>4</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="30"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="28">
+      <c r="A10" s="23">
         <v>5</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="28">
+      <c r="A11" s="23">
         <v>6</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="30"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="28">
+      <c r="A12" s="23">
         <v>7</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
-    </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1">
-      <c r="A13" s="31">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A13" s="26">
         <v>8</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -5670,21 +6444,21 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="15.6">
-      <c r="A15" s="64" t="s">
+    <row r="15" spans="1:11" ht="15.75">
+      <c r="A15" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="66"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="82"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -5696,148 +6470,148 @@
       <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="68" t="s">
+      <c r="E16" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="71"/>
-      <c r="G16" s="68" t="s">
+      <c r="F16" s="86"/>
+      <c r="G16" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="69"/>
-      <c r="I16" s="70"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="85"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="26">
+      <c r="A17" s="21">
         <v>1</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="57"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="78"/>
       <c r="K17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="26">
+      <c r="A18" s="21">
         <v>2</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="57"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="78"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="26">
+      <c r="A19" s="21">
         <v>3</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="57"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="78"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="26">
+      <c r="A20" s="21">
         <v>4</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="57"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="78"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="26">
+      <c r="A21" s="21">
         <v>5</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="57"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="78"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="26">
+      <c r="A22" s="21">
         <v>6</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="57"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="78"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="26">
+      <c r="A23" s="21">
         <v>7</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="57"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="78"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="26">
+      <c r="A24" s="21">
         <v>8</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="57"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="78"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="26">
+      <c r="A25" s="21">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
-    </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1">
-      <c r="A26" s="27">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="71"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A26" s="22">
         <v>10</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="54"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="28">
@@ -5880,271 +6654,271 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="49.95" customHeight="1">
-      <c r="A1" s="72" t="s">
+    <row r="1" spans="1:17" ht="49.9" customHeight="1">
+      <c r="A1" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="74"/>
-    </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
-      <c r="A2" s="75" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="89"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A2" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="91"/>
+      <c r="C2" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="77" t="s">
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="78"/>
-    </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1"/>
-    <row r="4" spans="1:17" ht="15.6">
-      <c r="A4" s="61" t="s">
+      <c r="I2" s="93"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="4" spans="1:17" ht="15.75">
+      <c r="A4" s="97" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="63"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="99"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="39" t="s">
+      <c r="I5" s="34" t="s">
         <v>66</v>
       </c>
       <c r="K5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="31.8">
-      <c r="A6" s="28">
+    <row r="6" spans="1:17" ht="34.5">
+      <c r="A6" s="23">
         <v>1</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="79" t="s">
+      <c r="K6" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="79"/>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="100"/>
+      <c r="O6" s="100"/>
+      <c r="P6" s="100"/>
+      <c r="Q6" s="100"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="28">
+      <c r="A7" s="23">
         <v>2</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="79" t="s">
+      <c r="K7" s="100" t="s">
         <v>126</v>
       </c>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="79"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="100"/>
+      <c r="P7" s="100"/>
+      <c r="Q7" s="100"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="28">
+      <c r="A8" s="23">
         <v>3</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="25" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="28">
+      <c r="A9" s="23">
         <v>4</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="30"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="28">
+      <c r="A10" s="23">
         <v>5</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="28">
+      <c r="A11" s="23">
         <v>6</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="30"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="28">
+      <c r="A12" s="23">
         <v>7</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1">
-      <c r="A13" s="31">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A13" s="26">
         <v>8</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:17" ht="15" thickBot="1">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" thickBot="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -6155,21 +6929,21 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15.6">
-      <c r="A15" s="64" t="s">
+    <row r="15" spans="1:17" ht="15.75">
+      <c r="A15" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="66"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="82"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -6181,181 +6955,181 @@
       <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="68" t="s">
+      <c r="E16" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="71"/>
-      <c r="G16" s="68" t="s">
+      <c r="F16" s="86"/>
+      <c r="G16" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="69"/>
-      <c r="I16" s="70"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="85"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="26">
+      <c r="A17" s="21">
         <v>1</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="80" t="s">
+      <c r="E17" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="81"/>
-      <c r="G17" s="80" t="s">
+      <c r="F17" s="102"/>
+      <c r="G17" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="82"/>
-      <c r="I17" s="83"/>
-    </row>
-    <row r="18" spans="1:11" ht="21.6">
-      <c r="A18" s="26">
+      <c r="H17" s="103"/>
+      <c r="I17" s="104"/>
+    </row>
+    <row r="18" spans="1:11" ht="23.25">
+      <c r="A18" s="21">
         <v>2</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="80" t="s">
+      <c r="E18" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="81"/>
-      <c r="G18" s="80" t="s">
+      <c r="F18" s="102"/>
+      <c r="G18" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="82"/>
-      <c r="I18" s="83"/>
-    </row>
-    <row r="19" spans="1:11" ht="31.8">
-      <c r="A19" s="26">
+      <c r="H18" s="103"/>
+      <c r="I18" s="104"/>
+    </row>
+    <row r="19" spans="1:11" ht="34.5">
+      <c r="A19" s="21">
         <v>3</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="80" t="s">
+      <c r="E19" s="101" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="81"/>
-      <c r="G19" s="80" t="s">
+      <c r="F19" s="102"/>
+      <c r="G19" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="H19" s="82"/>
-      <c r="I19" s="83"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="104"/>
       <c r="K19" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="26">
+      <c r="A20" s="21">
         <v>4</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="57"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="78"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="26">
+      <c r="A21" s="21">
         <v>5</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="57"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="78"/>
       <c r="K21" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="26">
+      <c r="A22" s="21">
         <v>6</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="57"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="78"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="26">
+      <c r="A23" s="21">
         <v>7</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="57"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="78"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="26">
+      <c r="A24" s="21">
         <v>8</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="57"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="78"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="26">
+      <c r="A25" s="21">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
-    </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1">
-      <c r="A26" s="27">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="71"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A26" s="22">
         <v>10</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="54"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -6398,125 +7172,135 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:C17"/>
+  <dimension ref="A5:C18"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:C17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="34.88671875" customWidth="1"/>
-    <col min="3" max="3" width="46.21875" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:3">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="106" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="36" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8">
-      <c r="A7" s="43" t="s">
+    <row r="7" spans="1:3" ht="30">
+      <c r="A7" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="37" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="57.6">
-      <c r="A8" s="43" t="s">
+    <row r="8" spans="1:3" ht="60">
+      <c r="A8" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="37" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8">
-      <c r="A9" s="43" t="s">
+    <row r="9" spans="1:3" ht="45">
+      <c r="A9" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="37" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.2">
-      <c r="A10" s="43" t="s">
+    <row r="10" spans="1:3" ht="45">
+      <c r="A10" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="37" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="107"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="106" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="85"/>
-    </row>
-    <row r="15" spans="1:3" ht="109.8" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="C14" s="106"/>
+    </row>
+    <row r="15" spans="1:3" ht="109.9" customHeight="1">
+      <c r="A15" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="105" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="84"/>
-    </row>
-    <row r="16" spans="1:3" ht="79.2" customHeight="1">
-      <c r="A16" s="43" t="s">
+      <c r="C15" s="105"/>
+    </row>
+    <row r="16" spans="1:3" ht="79.150000000000006" customHeight="1">
+      <c r="A16" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="105" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="84"/>
+      <c r="C16" s="105"/>
     </row>
     <row r="17" spans="1:3" ht="87" customHeight="1">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="105" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="84"/>
+      <c r="C17" s="105"/>
+    </row>
+    <row r="18" spans="1:3" ht="96.75" customHeight="1">
+      <c r="A18" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="105" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="105"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="B15:C15"/>
@@ -6525,6 +7309,7 @@
     <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6533,12 +7318,12 @@
   <dimension ref="B2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
@@ -6554,7 +7339,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="7.2" customHeight="1"/>
+    <row r="4" spans="2:3" ht="7.15" customHeight="1"/>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
chg: Updated intro brief, CJTF OPORDER, target list
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
+++ b/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="251">
   <si>
     <t>OP ACTIVE RESOLVE TARGET LIST</t>
   </si>
@@ -766,6 +766,27 @@
   </si>
   <si>
     <t>Homs</t>
+  </si>
+  <si>
+    <t>Rocket motor facility</t>
+  </si>
+  <si>
+    <t>SCUD / MLRS</t>
+  </si>
+  <si>
+    <t>MLRS and SCUD rocket engines. Repair and construction of rocket engines</t>
+  </si>
+  <si>
+    <t>Rocket research facility</t>
+  </si>
+  <si>
+    <t>Research into rockets</t>
+  </si>
+  <si>
+    <t>Syrian Intelligence Agency</t>
+  </si>
+  <si>
+    <t>Syrian Intelligence Agency HQ building</t>
   </si>
 </sst>
 </file>
@@ -1475,6 +1496,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1483,6 +1539,63 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1523,62 +1636,8 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1592,9 +1651,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1603,41 +1659,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2571,8 +2592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2593,24 +2614,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="49.95" customHeight="1" thickBot="1">
-      <c r="A1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="52" t="s">
+      <c r="A1" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="54"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="69"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3492,31 +3513,31 @@
       <c r="N28" s="44"/>
     </row>
     <row r="29" spans="1:14" ht="15" thickBot="1">
-      <c r="A29" s="95" t="s">
+      <c r="A29" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="96" t="s">
+      <c r="B29" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="96"/>
-      <c r="F29" s="96"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="96" t="s">
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="I29" s="98"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="100" t="str">
+      <c r="I29" s="55"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="57" t="str">
         <f t="shared" si="0"/>
         <v>OPARTGT026</v>
       </c>
-      <c r="L29" s="101" t="str">
+      <c r="L29" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Vehicle factory</v>
       </c>
-      <c r="M29" s="101">
+      <c r="M29" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4372,7 +4393,7 @@
       <c r="N58" s="44"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="108" t="s">
+      <c r="A59" s="65" t="s">
         <v>167</v>
       </c>
       <c r="B59" s="8" t="s">
@@ -4403,7 +4424,7 @@
       <c r="N59" s="44"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="109" t="s">
+      <c r="A60" s="66" t="s">
         <v>168</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -4432,10 +4453,10 @@
       <c r="N60" s="44"/>
     </row>
     <row r="61" spans="1:14" ht="24">
-      <c r="A61" s="108" t="s">
+      <c r="A61" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="B61" s="102" t="s">
+      <c r="B61" s="59" t="s">
         <v>238</v>
       </c>
       <c r="C61" s="47"/>
@@ -4450,7 +4471,7 @@
         <f t="shared" si="6"/>
         <v>OPARTGT058</v>
       </c>
-      <c r="L61" s="103" t="str">
+      <c r="L61" s="60" t="str">
         <f t="shared" si="7"/>
         <v>XXX Chemical Weapon research facility</v>
       </c>
@@ -4461,10 +4482,10 @@
       <c r="N61" s="44"/>
     </row>
     <row r="62" spans="1:14" ht="24.6" thickBot="1">
-      <c r="A62" s="108" t="s">
+      <c r="A62" s="65" t="s">
         <v>170</v>
       </c>
-      <c r="B62" s="102" t="s">
+      <c r="B62" s="59" t="s">
         <v>238</v>
       </c>
       <c r="C62" s="48"/>
@@ -4479,7 +4500,7 @@
         <f t="shared" si="6"/>
         <v>OPARTGT059</v>
       </c>
-      <c r="L62" s="103" t="str">
+      <c r="L62" s="60" t="str">
         <f t="shared" si="7"/>
         <v>XXX Chemical Weapon research facility</v>
       </c>
@@ -4490,10 +4511,10 @@
       <c r="N62" s="46"/>
     </row>
     <row r="63" spans="1:14" ht="24">
-      <c r="A63" s="108" t="s">
+      <c r="A63" s="65" t="s">
         <v>171</v>
       </c>
-      <c r="B63" s="102" t="s">
+      <c r="B63" s="59" t="s">
         <v>239</v>
       </c>
       <c r="C63" s="1"/>
@@ -4506,7 +4527,7 @@
         <f t="shared" si="6"/>
         <v>OPARTGT060</v>
       </c>
-      <c r="L63" s="103" t="str">
+      <c r="L63" s="60" t="str">
         <f t="shared" si="7"/>
         <v>XXX Chemical Weapon production facility</v>
       </c>
@@ -4516,10 +4537,10 @@
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="108" t="s">
+      <c r="A64" s="65" t="s">
         <v>172</v>
       </c>
-      <c r="B64" s="102" t="s">
+      <c r="B64" s="59" t="s">
         <v>240</v>
       </c>
       <c r="C64" s="1"/>
@@ -4532,7 +4553,7 @@
         <f t="shared" si="6"/>
         <v>OPARTGT061</v>
       </c>
-      <c r="L64" s="103" t="str">
+      <c r="L64" s="60" t="str">
         <f t="shared" si="7"/>
         <v>XXX Chemical Weapon Storage</v>
       </c>
@@ -4542,10 +4563,10 @@
       </c>
     </row>
     <row r="65" spans="1:14" ht="28.8">
-      <c r="A65" s="108" t="s">
+      <c r="A65" s="65" t="s">
         <v>173</v>
       </c>
-      <c r="B65" s="105" t="s">
+      <c r="B65" s="62" t="s">
         <v>241</v>
       </c>
       <c r="C65" s="1"/>
@@ -4556,11 +4577,11 @@
       <c r="H65" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="K65" s="107" t="str">
+      <c r="K65" s="64" t="str">
         <f t="shared" ref="K65:K103" si="9">A65</f>
         <v>OPARTGT062</v>
       </c>
-      <c r="L65" s="106" t="str">
+      <c r="L65" s="63" t="str">
         <f t="shared" ref="L65:L103" si="10">B65</f>
         <v>Air Defence Acadamey</v>
       </c>
@@ -4568,7 +4589,7 @@
         <f t="shared" ref="M65:M103" si="11">C65</f>
         <v>0</v>
       </c>
-      <c r="N65" s="104" t="s">
+      <c r="N65" s="61" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4576,32 +4597,40 @@
       <c r="A66" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B66" s="102"/>
+      <c r="B66" s="59" t="s">
+        <v>244</v>
+      </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-      <c r="H66" s="8"/>
+      <c r="H66" s="8" t="s">
+        <v>245</v>
+      </c>
       <c r="K66" s="49" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT063</v>
       </c>
-      <c r="L66" s="103">
+      <c r="L66" s="60" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>Rocket motor facility</v>
       </c>
       <c r="M66" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N66" s="104"/>
+      <c r="N66" s="61" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="67" spans="1:14">
       <c r="A67" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B67" s="102"/>
+      <c r="B67" s="59" t="s">
+        <v>247</v>
+      </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -4612,21 +4641,25 @@
         <f t="shared" si="9"/>
         <v>OPARTGT064</v>
       </c>
-      <c r="L67" s="103">
+      <c r="L67" s="60" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>Rocket research facility</v>
       </c>
       <c r="M67" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N67" s="104"/>
+      <c r="N67" s="61" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="68" spans="1:14">
       <c r="A68" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B68" s="102"/>
+      <c r="B68" s="59" t="s">
+        <v>249</v>
+      </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -4637,21 +4670,23 @@
         <f t="shared" si="9"/>
         <v>OPARTGT065</v>
       </c>
-      <c r="L68" s="103">
+      <c r="L68" s="60" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>Syrian Intelligence Agency</v>
       </c>
       <c r="M68" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N68" s="104"/>
+      <c r="N68" s="61" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="69" spans="1:14">
       <c r="A69" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B69" s="102"/>
+      <c r="B69" s="59"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -4662,7 +4697,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT066</v>
       </c>
-      <c r="L69" s="103">
+      <c r="L69" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4670,13 +4705,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N69" s="104"/>
+      <c r="N69" s="61"/>
     </row>
     <row r="70" spans="1:14">
       <c r="A70" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B70" s="102"/>
+      <c r="B70" s="59"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -4687,7 +4722,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT067</v>
       </c>
-      <c r="L70" s="103">
+      <c r="L70" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4695,13 +4730,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N70" s="104"/>
+      <c r="N70" s="61"/>
     </row>
     <row r="71" spans="1:14">
       <c r="A71" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B71" s="102"/>
+      <c r="B71" s="59"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -4712,7 +4747,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT068</v>
       </c>
-      <c r="L71" s="103">
+      <c r="L71" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4720,13 +4755,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N71" s="104"/>
+      <c r="N71" s="61"/>
     </row>
     <row r="72" spans="1:14">
       <c r="A72" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B72" s="102"/>
+      <c r="B72" s="59"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -4737,7 +4772,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT069</v>
       </c>
-      <c r="L72" s="103">
+      <c r="L72" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4745,13 +4780,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N72" s="104"/>
+      <c r="N72" s="61"/>
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B73" s="102"/>
+      <c r="B73" s="59"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -4762,7 +4797,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT070</v>
       </c>
-      <c r="L73" s="103">
+      <c r="L73" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4770,13 +4805,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N73" s="104"/>
+      <c r="N73" s="61"/>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B74" s="102"/>
+      <c r="B74" s="59"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -4787,7 +4822,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT071</v>
       </c>
-      <c r="L74" s="103">
+      <c r="L74" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4795,13 +4830,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N74" s="104"/>
+      <c r="N74" s="61"/>
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B75" s="102"/>
+      <c r="B75" s="59"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -4812,7 +4847,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT072</v>
       </c>
-      <c r="L75" s="103">
+      <c r="L75" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4820,13 +4855,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N75" s="104"/>
+      <c r="N75" s="61"/>
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B76" s="102"/>
+      <c r="B76" s="59"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -4837,7 +4872,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT073</v>
       </c>
-      <c r="L76" s="103">
+      <c r="L76" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4845,13 +4880,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N76" s="104"/>
+      <c r="N76" s="61"/>
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B77" s="102"/>
+      <c r="B77" s="59"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -4862,7 +4897,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT074</v>
       </c>
-      <c r="L77" s="103">
+      <c r="L77" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4870,13 +4905,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N77" s="104"/>
+      <c r="N77" s="61"/>
     </row>
     <row r="78" spans="1:14">
       <c r="A78" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B78" s="102"/>
+      <c r="B78" s="59"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -4887,7 +4922,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT075</v>
       </c>
-      <c r="L78" s="103">
+      <c r="L78" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4895,13 +4930,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N78" s="104"/>
+      <c r="N78" s="61"/>
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B79" s="102"/>
+      <c r="B79" s="59"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -4912,7 +4947,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT076</v>
       </c>
-      <c r="L79" s="103">
+      <c r="L79" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4920,13 +4955,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N79" s="104"/>
+      <c r="N79" s="61"/>
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B80" s="102"/>
+      <c r="B80" s="59"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -4937,7 +4972,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT077</v>
       </c>
-      <c r="L80" s="103">
+      <c r="L80" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4945,13 +4980,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N80" s="104"/>
+      <c r="N80" s="61"/>
     </row>
     <row r="81" spans="1:14">
       <c r="A81" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B81" s="102"/>
+      <c r="B81" s="59"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -4962,7 +4997,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT078</v>
       </c>
-      <c r="L81" s="103">
+      <c r="L81" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4970,13 +5005,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N81" s="104"/>
+      <c r="N81" s="61"/>
     </row>
     <row r="82" spans="1:14">
       <c r="A82" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B82" s="102"/>
+      <c r="B82" s="59"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -4987,7 +5022,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT079</v>
       </c>
-      <c r="L82" s="103">
+      <c r="L82" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -4995,13 +5030,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N82" s="104"/>
+      <c r="N82" s="61"/>
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="102"/>
+      <c r="B83" s="59"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -5012,7 +5047,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT080</v>
       </c>
-      <c r="L83" s="103">
+      <c r="L83" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5020,13 +5055,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N83" s="104"/>
+      <c r="N83" s="61"/>
     </row>
     <row r="84" spans="1:14">
       <c r="A84" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B84" s="102"/>
+      <c r="B84" s="59"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -5037,7 +5072,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT081</v>
       </c>
-      <c r="L84" s="103">
+      <c r="L84" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5045,13 +5080,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N84" s="104"/>
+      <c r="N84" s="61"/>
     </row>
     <row r="85" spans="1:14">
       <c r="A85" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="B85" s="102"/>
+      <c r="B85" s="59"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -5062,7 +5097,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT082</v>
       </c>
-      <c r="L85" s="103">
+      <c r="L85" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5070,13 +5105,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N85" s="104"/>
+      <c r="N85" s="61"/>
     </row>
     <row r="86" spans="1:14">
       <c r="A86" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B86" s="102"/>
+      <c r="B86" s="59"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -5087,7 +5122,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT083</v>
       </c>
-      <c r="L86" s="103">
+      <c r="L86" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5095,13 +5130,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N86" s="104"/>
+      <c r="N86" s="61"/>
     </row>
     <row r="87" spans="1:14">
       <c r="A87" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="B87" s="102"/>
+      <c r="B87" s="59"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -5112,7 +5147,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT084</v>
       </c>
-      <c r="L87" s="103">
+      <c r="L87" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5120,13 +5155,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N87" s="104"/>
+      <c r="N87" s="61"/>
     </row>
     <row r="88" spans="1:14">
       <c r="A88" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="B88" s="102"/>
+      <c r="B88" s="59"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -5137,7 +5172,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT085</v>
       </c>
-      <c r="L88" s="103">
+      <c r="L88" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5145,13 +5180,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N88" s="104"/>
+      <c r="N88" s="61"/>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B89" s="102"/>
+      <c r="B89" s="59"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -5162,7 +5197,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT086</v>
       </c>
-      <c r="L89" s="103">
+      <c r="L89" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5170,13 +5205,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N89" s="104"/>
+      <c r="N89" s="61"/>
     </row>
     <row r="90" spans="1:14">
       <c r="A90" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B90" s="102"/>
+      <c r="B90" s="59"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -5187,7 +5222,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT087</v>
       </c>
-      <c r="L90" s="103">
+      <c r="L90" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5195,13 +5230,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N90" s="104"/>
+      <c r="N90" s="61"/>
     </row>
     <row r="91" spans="1:14">
       <c r="A91" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B91" s="102"/>
+      <c r="B91" s="59"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -5212,7 +5247,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT088</v>
       </c>
-      <c r="L91" s="103">
+      <c r="L91" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5220,13 +5255,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N91" s="104"/>
+      <c r="N91" s="61"/>
     </row>
     <row r="92" spans="1:14">
       <c r="A92" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B92" s="102"/>
+      <c r="B92" s="59"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -5237,7 +5272,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT089</v>
       </c>
-      <c r="L92" s="103">
+      <c r="L92" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5245,13 +5280,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N92" s="104"/>
+      <c r="N92" s="61"/>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B93" s="102"/>
+      <c r="B93" s="59"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -5262,7 +5297,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT090</v>
       </c>
-      <c r="L93" s="103">
+      <c r="L93" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5270,13 +5305,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N93" s="104"/>
+      <c r="N93" s="61"/>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B94" s="102"/>
+      <c r="B94" s="59"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -5287,7 +5322,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT091</v>
       </c>
-      <c r="L94" s="103">
+      <c r="L94" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5295,13 +5330,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N94" s="104"/>
+      <c r="N94" s="61"/>
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B95" s="102"/>
+      <c r="B95" s="59"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -5312,7 +5347,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT092</v>
       </c>
-      <c r="L95" s="103">
+      <c r="L95" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5320,13 +5355,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N95" s="104"/>
+      <c r="N95" s="61"/>
     </row>
     <row r="96" spans="1:14">
       <c r="A96" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B96" s="102"/>
+      <c r="B96" s="59"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -5337,7 +5372,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT093</v>
       </c>
-      <c r="L96" s="103">
+      <c r="L96" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5345,13 +5380,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N96" s="104"/>
+      <c r="N96" s="61"/>
     </row>
     <row r="97" spans="1:14">
       <c r="A97" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B97" s="102"/>
+      <c r="B97" s="59"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -5362,7 +5397,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT094</v>
       </c>
-      <c r="L97" s="103">
+      <c r="L97" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5370,13 +5405,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N97" s="104"/>
+      <c r="N97" s="61"/>
     </row>
     <row r="98" spans="1:14">
       <c r="A98" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B98" s="102"/>
+      <c r="B98" s="59"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -5387,7 +5422,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT095</v>
       </c>
-      <c r="L98" s="103">
+      <c r="L98" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5395,13 +5430,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N98" s="104"/>
+      <c r="N98" s="61"/>
     </row>
     <row r="99" spans="1:14">
       <c r="A99" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B99" s="102"/>
+      <c r="B99" s="59"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -5412,7 +5447,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT096</v>
       </c>
-      <c r="L99" s="103">
+      <c r="L99" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5420,13 +5455,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N99" s="104"/>
+      <c r="N99" s="61"/>
     </row>
     <row r="100" spans="1:14">
       <c r="A100" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B100" s="102"/>
+      <c r="B100" s="59"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -5437,7 +5472,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT097</v>
       </c>
-      <c r="L100" s="103">
+      <c r="L100" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5445,13 +5480,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N100" s="104"/>
+      <c r="N100" s="61"/>
     </row>
     <row r="101" spans="1:14">
       <c r="A101" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B101" s="102"/>
+      <c r="B101" s="59"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -5462,7 +5497,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT098</v>
       </c>
-      <c r="L101" s="103">
+      <c r="L101" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5470,13 +5505,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N101" s="104"/>
+      <c r="N101" s="61"/>
     </row>
     <row r="102" spans="1:14">
       <c r="A102" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B102" s="102"/>
+      <c r="B102" s="59"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -5487,7 +5522,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT099</v>
       </c>
-      <c r="L102" s="103">
+      <c r="L102" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5495,13 +5530,13 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N102" s="104"/>
+      <c r="N102" s="61"/>
     </row>
     <row r="103" spans="1:14">
       <c r="A103" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="B103" s="102"/>
+      <c r="B103" s="59"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -5512,7 +5547,7 @@
         <f t="shared" si="9"/>
         <v>OPARTGT100</v>
       </c>
-      <c r="L103" s="103">
+      <c r="L103" s="60">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5520,7 +5555,7 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N103" s="104"/>
+      <c r="N103" s="61"/>
     </row>
     <row r="104" spans="1:14">
       <c r="A104" s="1"/>
@@ -7694,34 +7729,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.95" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="57"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="91"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="59"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="95"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1">
       <c r="K3" t="s">
@@ -7729,17 +7764,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.6">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="99" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="67"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="101"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="33" t="s">
@@ -7886,17 +7921,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15.6">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="70"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="84"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="20" t="s">
@@ -7911,15 +7946,15 @@
       <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="73" t="s">
+      <c r="E16" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="78"/>
-      <c r="G16" s="73" t="s">
+      <c r="F16" s="88"/>
+      <c r="G16" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="74"/>
-      <c r="I16" s="75"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="87"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="21">
@@ -7928,11 +7963,11 @@
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="77"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
       <c r="K17" t="s">
         <v>68</v>
       </c>
@@ -7944,11 +7979,11 @@
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="77"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="80"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="21">
@@ -7957,11 +7992,11 @@
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="77"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="80"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="21">
@@ -7970,11 +8005,11 @@
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="77"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="80"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="21">
@@ -7983,11 +8018,11 @@
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="77"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="80"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="21">
@@ -7996,11 +8031,11 @@
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="77"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="80"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="21">
@@ -8009,11 +8044,11 @@
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="77"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="80"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="21">
@@ -8022,11 +8057,11 @@
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="77"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="80"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="21">
@@ -8035,11 +8070,11 @@
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="82"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="22">
@@ -8048,23 +8083,19 @@
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="86"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A4:I4"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
@@ -8079,11 +8110,15 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8112,50 +8147,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.95" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="57"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="91"/>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="59"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="60" t="s">
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="61"/>
+      <c r="I2" s="95"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.6">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="99" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="67"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="101"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="33" t="s">
@@ -8217,15 +8252,15 @@
       <c r="I6" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="91" t="s">
+      <c r="K6" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="102"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="23">
@@ -8255,15 +8290,15 @@
       <c r="I7" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="91" t="s">
+      <c r="K7" s="102" t="s">
         <v>126</v>
       </c>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
-      <c r="O7" s="91"/>
-      <c r="P7" s="91"/>
-      <c r="Q7" s="91"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="102"/>
+      <c r="P7" s="102"/>
+      <c r="Q7" s="102"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="23">
@@ -8371,17 +8406,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="15.6">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="70"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="84"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="20" t="s">
@@ -8396,15 +8431,15 @@
       <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="73" t="s">
+      <c r="E16" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="78"/>
-      <c r="G16" s="73" t="s">
+      <c r="F16" s="88"/>
+      <c r="G16" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="74"/>
-      <c r="I16" s="75"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="87"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="21">
@@ -8419,15 +8454,15 @@
       <c r="D17" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="87" t="s">
+      <c r="E17" s="103" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="88"/>
-      <c r="G17" s="87" t="s">
+      <c r="F17" s="104"/>
+      <c r="G17" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="89"/>
-      <c r="I17" s="90"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="106"/>
     </row>
     <row r="18" spans="1:11" ht="21.6">
       <c r="A18" s="21">
@@ -8442,15 +8477,15 @@
       <c r="D18" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="87" t="s">
+      <c r="E18" s="103" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="88"/>
-      <c r="G18" s="87" t="s">
+      <c r="F18" s="104"/>
+      <c r="G18" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="89"/>
-      <c r="I18" s="90"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="106"/>
     </row>
     <row r="19" spans="1:11" ht="31.8">
       <c r="A19" s="21">
@@ -8465,15 +8500,15 @@
       <c r="D19" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="87" t="s">
+      <c r="E19" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="88"/>
-      <c r="G19" s="87" t="s">
+      <c r="F19" s="104"/>
+      <c r="G19" s="103" t="s">
         <v>104</v>
       </c>
-      <c r="H19" s="89"/>
-      <c r="I19" s="90"/>
+      <c r="H19" s="105"/>
+      <c r="I19" s="106"/>
       <c r="K19" t="s">
         <v>68</v>
       </c>
@@ -8485,11 +8520,11 @@
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="77"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="80"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="21">
@@ -8498,11 +8533,11 @@
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="77"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="80"/>
       <c r="K21" t="s">
         <v>93</v>
       </c>
@@ -8514,11 +8549,11 @@
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="77"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="80"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="21">
@@ -8527,11 +8562,11 @@
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="77"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="80"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="21">
@@ -8540,11 +8575,11 @@
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="77"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="80"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="21">
@@ -8553,11 +8588,11 @@
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="82"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="22">
@@ -8566,14 +8601,28 @@
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="86"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="K6:Q6"/>
@@ -8590,20 +8639,6 @@
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:I20"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8626,11 +8661,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:3">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="36" t="s">
@@ -8688,56 +8723,56 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="109" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="109"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="93"/>
+      <c r="C14" s="108"/>
     </row>
     <row r="15" spans="1:3" ht="109.95" customHeight="1">
       <c r="A15" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="92"/>
+      <c r="C15" s="107"/>
     </row>
     <row r="16" spans="1:3" ht="79.2" customHeight="1">
       <c r="A16" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="107" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="92"/>
+      <c r="C16" s="107"/>
     </row>
     <row r="17" spans="1:3" ht="87" customHeight="1">
       <c r="A17" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="107" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="92"/>
+      <c r="C17" s="107"/>
     </row>
     <row r="18" spans="1:3" ht="96.75" customHeight="1">
       <c r="A18" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="C18" s="92"/>
+      <c r="C18" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
chg: Added target category explanation
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
+++ b/INTELLIGENCE/OPAR_TARGET_LIST.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18492" windowHeight="11700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Target list" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <sheet name="Explanation Target Effetcs" sheetId="9" r:id="rId7"/>
     <sheet name="Example_support" sheetId="4" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="290">
   <si>
     <t>OP ACTIVE RESOLVE TARGET LIST</t>
   </si>
@@ -829,6 +829,81 @@
   </si>
   <si>
     <t>EFFECT</t>
+  </si>
+  <si>
+    <t>Syrian Broadcasting Headquarter</t>
+  </si>
+  <si>
+    <t>Used for propaganda, and for spreading the message for the Syrian regime</t>
+  </si>
+  <si>
+    <t>Naval Base</t>
+  </si>
+  <si>
+    <t>Nuclear weapons</t>
+  </si>
+  <si>
+    <t>Chemical weapons</t>
+  </si>
+  <si>
+    <t>Biological weapons</t>
+  </si>
+  <si>
+    <t>Command, Control and Communications</t>
+  </si>
+  <si>
+    <t>Airforces and airfields</t>
+  </si>
+  <si>
+    <t>Air Defence</t>
+  </si>
+  <si>
+    <t>Ground forces and facilities</t>
+  </si>
+  <si>
+    <t>Naval forces and ports</t>
+  </si>
+  <si>
+    <t>Military supply and storage</t>
+  </si>
+  <si>
+    <t>Transportation / lines of communications</t>
+  </si>
+  <si>
+    <t>Political leadership</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Petroleum industry</t>
+  </si>
+  <si>
+    <t>Fuel production</t>
+  </si>
+  <si>
+    <t>Fuel storage</t>
+  </si>
+  <si>
+    <t>Pipelines</t>
+  </si>
+  <si>
+    <t>Electric power</t>
+  </si>
+  <si>
+    <t>Powerplants, powerlines</t>
+  </si>
+  <si>
+    <t>Ammunition storage, warehouses, factories</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>General industry not covered by other categories</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1542,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1601,6 +1676,35 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1609,6 +1713,63 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1649,62 +1810,8 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1718,46 +1825,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2074,16 +2155,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>706755</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2101,8 +2182,55 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5467350" y="19050"/>
-          <a:ext cx="3505200" cy="7058025"/>
+          <a:off x="7945755" y="175260"/>
+          <a:ext cx="3657600" cy="6800850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>150242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2049" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9144000" y="1285622"/>
+          <a:ext cx="5052060" cy="3682618"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2941,48 +3069,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N317"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="78.42578125" customWidth="1"/>
+    <col min="14" max="14" width="78.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="49.9" customHeight="1" thickBot="1">
-      <c r="A1" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="61" t="s">
+    <row r="1" spans="1:14" ht="49.95" customHeight="1" thickBot="1">
+      <c r="A1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="63"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1">
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="74"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
@@ -3002,14 +3130,14 @@
       <c r="M2" s="40"/>
       <c r="N2" s="41"/>
     </row>
-    <row r="3" spans="1:14" ht="29.45" customHeight="1" thickBot="1">
+    <row r="3" spans="1:14" ht="29.4" customHeight="1" thickBot="1">
       <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>62</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3085,7 +3213,7 @@
         <f>C4</f>
         <v>SCUDs</v>
       </c>
-      <c r="N4" s="103" t="s">
+      <c r="N4" s="61" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3128,7 +3256,7 @@
         <f t="shared" ref="M5:M29" si="2">C5</f>
         <v>SCUDs</v>
       </c>
-      <c r="N5" s="104" t="s">
+      <c r="N5" s="62" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3167,7 +3295,7 @@
         <f t="shared" si="2"/>
         <v>MLRS</v>
       </c>
-      <c r="N6" s="104" t="s">
+      <c r="N6" s="62" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3206,7 +3334,7 @@
         <f t="shared" si="2"/>
         <v>MLRS</v>
       </c>
-      <c r="N7" s="104" t="s">
+      <c r="N7" s="62" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3245,7 +3373,7 @@
         <f t="shared" si="2"/>
         <v>MLRS</v>
       </c>
-      <c r="N8" s="104" t="s">
+      <c r="N8" s="62" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3284,7 +3412,7 @@
         <f t="shared" si="2"/>
         <v>MLRS</v>
       </c>
-      <c r="N9" s="104" t="s">
+      <c r="N9" s="62" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3317,7 +3445,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N10" s="104"/>
+      <c r="N10" s="62"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="7" t="s">
@@ -3348,7 +3476,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N11" s="104"/>
+      <c r="N11" s="62"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="7" t="s">
@@ -3379,7 +3507,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N12" s="104"/>
+      <c r="N12" s="62"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="7" t="s">
@@ -3410,7 +3538,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N13" s="104"/>
+      <c r="N13" s="62"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="7" t="s">
@@ -3441,7 +3569,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N14" s="104"/>
+      <c r="N14" s="62"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="7" t="s">
@@ -3472,7 +3600,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N15" s="104"/>
+      <c r="N15" s="62"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="7" t="s">
@@ -3503,7 +3631,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N16" s="104"/>
+      <c r="N16" s="62"/>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="7" t="s">
@@ -3534,7 +3662,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N17" s="104"/>
+      <c r="N17" s="62"/>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="7" t="s">
@@ -3565,7 +3693,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N18" s="104"/>
+      <c r="N18" s="62"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="7" t="s">
@@ -3596,7 +3724,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N19" s="104"/>
+      <c r="N19" s="62"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="7" t="s">
@@ -3627,7 +3755,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N20" s="104"/>
+      <c r="N20" s="62"/>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="7" t="s">
@@ -3658,7 +3786,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N21" s="104"/>
+      <c r="N21" s="62"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="7" t="s">
@@ -3687,7 +3815,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N22" s="104"/>
+      <c r="N22" s="62"/>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="7" t="s">
@@ -3716,7 +3844,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N23" s="104"/>
+      <c r="N23" s="62"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="7" t="s">
@@ -3747,7 +3875,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N24" s="104"/>
+      <c r="N24" s="62"/>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="7" t="s">
@@ -3778,7 +3906,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N25" s="104"/>
+      <c r="N25" s="62"/>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="7" t="s">
@@ -3809,7 +3937,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N26" s="104"/>
+      <c r="N26" s="62"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="7" t="s">
@@ -3840,7 +3968,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N27" s="104"/>
+      <c r="N27" s="62"/>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="7" t="s">
@@ -3871,9 +3999,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N28" s="104"/>
-    </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1">
+      <c r="N28" s="62"/>
+    </row>
+    <row r="29" spans="1:14" ht="15" thickBot="1">
       <c r="A29" s="46" t="s">
         <v>38</v>
       </c>
@@ -3902,7 +4030,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N29" s="105"/>
+      <c r="N29" s="63"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="13" t="s">
@@ -3933,7 +4061,7 @@
         <f>C30</f>
         <v>0</v>
       </c>
-      <c r="N30" s="103"/>
+      <c r="N30" s="61"/>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="7" t="s">
@@ -3964,7 +4092,7 @@
         <f t="shared" ref="M31" si="5">C31</f>
         <v>0</v>
       </c>
-      <c r="N31" s="104"/>
+      <c r="N31" s="62"/>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="13" t="s">
@@ -3995,7 +4123,7 @@
         <f>C32</f>
         <v>0</v>
       </c>
-      <c r="N32" s="104"/>
+      <c r="N32" s="62"/>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="7" t="s">
@@ -4024,7 +4152,7 @@
         <f t="shared" ref="M33:M64" si="8">C33</f>
         <v>0</v>
       </c>
-      <c r="N33" s="104"/>
+      <c r="N33" s="62"/>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="7" t="s">
@@ -4053,7 +4181,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N34" s="104"/>
+      <c r="N34" s="62"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="7" t="s">
@@ -4082,7 +4210,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N35" s="104"/>
+      <c r="N35" s="62"/>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="7" t="s">
@@ -4111,7 +4239,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N36" s="104"/>
+      <c r="N36" s="62"/>
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="7" t="s">
@@ -4140,9 +4268,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N37" s="104"/>
-    </row>
-    <row r="38" spans="1:14" ht="30">
+      <c r="N37" s="62"/>
+    </row>
+    <row r="38" spans="1:14" ht="28.8">
       <c r="A38" s="7" t="s">
         <v>136</v>
       </c>
@@ -4169,7 +4297,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N38" s="104" t="s">
+      <c r="N38" s="62" t="s">
         <v>249</v>
       </c>
     </row>
@@ -4200,7 +4328,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N39" s="104"/>
+      <c r="N39" s="62"/>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="7" t="s">
@@ -4229,7 +4357,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N40" s="104"/>
+      <c r="N40" s="62"/>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="7" t="s">
@@ -4258,7 +4386,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N41" s="104"/>
+      <c r="N41" s="62"/>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="7" t="s">
@@ -4287,7 +4415,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N42" s="104"/>
+      <c r="N42" s="62"/>
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="7" t="s">
@@ -4316,7 +4444,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N43" s="104"/>
+      <c r="N43" s="62"/>
     </row>
     <row r="44" spans="1:14">
       <c r="A44" s="7" t="s">
@@ -4345,7 +4473,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N44" s="104"/>
+      <c r="N44" s="62"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="7" t="s">
@@ -4374,7 +4502,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N45" s="104"/>
+      <c r="N45" s="62"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="7" t="s">
@@ -4405,7 +4533,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N46" s="104"/>
+      <c r="N46" s="62"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="7" t="s">
@@ -4434,7 +4562,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N47" s="104"/>
+      <c r="N47" s="62"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="7" t="s">
@@ -4463,7 +4591,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N48" s="104"/>
+      <c r="N48" s="62"/>
     </row>
     <row r="49" spans="1:14">
       <c r="A49" s="7" t="s">
@@ -4492,7 +4620,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N49" s="104"/>
+      <c r="N49" s="62"/>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="7" t="s">
@@ -4521,7 +4649,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N50" s="104"/>
+      <c r="N50" s="62"/>
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="7" t="s">
@@ -4550,7 +4678,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N51" s="104"/>
+      <c r="N51" s="62"/>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" s="7" t="s">
@@ -4579,7 +4707,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N52" s="104"/>
+      <c r="N52" s="62"/>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="7" t="s">
@@ -4608,7 +4736,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N53" s="104"/>
+      <c r="N53" s="62"/>
     </row>
     <row r="54" spans="1:14">
       <c r="A54" s="7" t="s">
@@ -4637,7 +4765,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N54" s="104"/>
+      <c r="N54" s="62"/>
     </row>
     <row r="55" spans="1:14">
       <c r="A55" s="7" t="s">
@@ -4666,7 +4794,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N55" s="104"/>
+      <c r="N55" s="62"/>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" s="9" t="s">
@@ -4695,7 +4823,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N56" s="104"/>
+      <c r="N56" s="62"/>
     </row>
     <row r="57" spans="1:14">
       <c r="A57" s="9" t="s">
@@ -4724,7 +4852,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N57" s="104"/>
+      <c r="N57" s="62"/>
     </row>
     <row r="58" spans="1:14">
       <c r="A58" s="9" t="s">
@@ -4753,7 +4881,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N58" s="104"/>
+      <c r="N58" s="62"/>
     </row>
     <row r="59" spans="1:14">
       <c r="A59" s="57" t="s">
@@ -4784,7 +4912,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N59" s="104"/>
+      <c r="N59" s="62"/>
     </row>
     <row r="60" spans="1:14">
       <c r="A60" s="58" t="s">
@@ -4813,9 +4941,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N60" s="104"/>
-    </row>
-    <row r="61" spans="1:14" ht="24.75">
+      <c r="N60" s="62"/>
+    </row>
+    <row r="61" spans="1:14" ht="24">
       <c r="A61" s="57" t="s">
         <v>159</v>
       </c>
@@ -4842,23 +4970,23 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N61" s="104"/>
-    </row>
-    <row r="62" spans="1:14" ht="24.75">
+      <c r="N61" s="62"/>
+    </row>
+    <row r="62" spans="1:14" ht="24">
       <c r="A62" s="57" t="s">
         <v>160</v>
       </c>
       <c r="B62" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="C62" s="107"/>
-      <c r="D62" s="107"/>
-      <c r="E62" s="107"/>
-      <c r="F62" s="107"/>
-      <c r="G62" s="107"/>
+      <c r="C62" s="65"/>
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="65"/>
+      <c r="G62" s="65"/>
       <c r="H62" s="8"/>
-      <c r="I62" s="110"/>
-      <c r="J62" s="110"/>
+      <c r="I62" s="68"/>
+      <c r="J62" s="68"/>
       <c r="K62" s="43" t="str">
         <f t="shared" si="6"/>
         <v>OPARTGT059</v>
@@ -4871,9 +4999,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N62" s="106"/>
-    </row>
-    <row r="63" spans="1:14" ht="24.75">
+      <c r="N62" s="64"/>
+    </row>
+    <row r="63" spans="1:14" ht="24">
       <c r="A63" s="57" t="s">
         <v>161</v>
       </c>
@@ -4888,7 +5016,7 @@
       <c r="H63" s="8"/>
       <c r="I63" s="38"/>
       <c r="J63" s="38"/>
-      <c r="K63" s="108" t="str">
+      <c r="K63" s="66" t="str">
         <f t="shared" si="6"/>
         <v>OPARTGT060</v>
       </c>
@@ -4917,7 +5045,7 @@
       <c r="H64" s="8"/>
       <c r="I64" s="38"/>
       <c r="J64" s="38"/>
-      <c r="K64" s="108" t="str">
+      <c r="K64" s="66" t="str">
         <f t="shared" si="6"/>
         <v>OPARTGT061</v>
       </c>
@@ -4931,7 +5059,7 @@
       </c>
       <c r="N64" s="29"/>
     </row>
-    <row r="65" spans="1:14" ht="45">
+    <row r="65" spans="1:14" ht="28.8">
       <c r="A65" s="57" t="s">
         <v>163</v>
       </c>
@@ -4948,7 +5076,7 @@
       </c>
       <c r="I65" s="38"/>
       <c r="J65" s="38"/>
-      <c r="K65" s="109" t="str">
+      <c r="K65" s="67" t="str">
         <f t="shared" ref="K65:K103" si="9">A65</f>
         <v>OPARTGT062</v>
       </c>
@@ -4981,7 +5109,7 @@
       </c>
       <c r="I66" s="38"/>
       <c r="J66" s="38"/>
-      <c r="K66" s="108" t="str">
+      <c r="K66" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT063</v>
       </c>
@@ -5012,7 +5140,7 @@
       <c r="H67" s="8"/>
       <c r="I67" s="38"/>
       <c r="J67" s="38"/>
-      <c r="K67" s="108" t="str">
+      <c r="K67" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT064</v>
       </c>
@@ -5043,7 +5171,7 @@
       <c r="H68" s="8"/>
       <c r="I68" s="38"/>
       <c r="J68" s="38"/>
-      <c r="K68" s="108" t="str">
+      <c r="K68" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT065</v>
       </c>
@@ -5074,7 +5202,7 @@
       <c r="H69" s="8"/>
       <c r="I69" s="38"/>
       <c r="J69" s="38"/>
-      <c r="K69" s="108" t="str">
+      <c r="K69" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT066</v>
       </c>
@@ -5105,7 +5233,7 @@
       <c r="H70" s="8"/>
       <c r="I70" s="38"/>
       <c r="J70" s="38"/>
-      <c r="K70" s="108" t="str">
+      <c r="K70" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT067</v>
       </c>
@@ -5136,7 +5264,7 @@
       <c r="H71" s="8"/>
       <c r="I71" s="38"/>
       <c r="J71" s="38"/>
-      <c r="K71" s="108" t="str">
+      <c r="K71" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT068</v>
       </c>
@@ -5167,7 +5295,7 @@
       <c r="H72" s="8"/>
       <c r="I72" s="38"/>
       <c r="J72" s="38"/>
-      <c r="K72" s="108" t="str">
+      <c r="K72" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT069</v>
       </c>
@@ -5187,7 +5315,9 @@
       <c r="A73" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B73" s="53"/>
+      <c r="B73" s="53" t="s">
+        <v>265</v>
+      </c>
       <c r="C73" s="42"/>
       <c r="D73" s="42"/>
       <c r="E73" s="42"/>
@@ -5196,19 +5326,21 @@
       <c r="H73" s="8"/>
       <c r="I73" s="38"/>
       <c r="J73" s="38"/>
-      <c r="K73" s="108" t="str">
+      <c r="K73" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT070</v>
       </c>
-      <c r="L73" s="54">
+      <c r="L73" s="54" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>Syrian Broadcasting Headquarter</v>
       </c>
       <c r="M73" s="44">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N73" s="29"/>
+      <c r="N73" s="29" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="7" t="s">
@@ -5223,7 +5355,7 @@
       <c r="H74" s="8"/>
       <c r="I74" s="38"/>
       <c r="J74" s="38"/>
-      <c r="K74" s="108" t="str">
+      <c r="K74" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT071</v>
       </c>
@@ -5250,7 +5382,7 @@
       <c r="H75" s="8"/>
       <c r="I75" s="38"/>
       <c r="J75" s="38"/>
-      <c r="K75" s="108" t="str">
+      <c r="K75" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT072</v>
       </c>
@@ -5277,7 +5409,7 @@
       <c r="H76" s="8"/>
       <c r="I76" s="38"/>
       <c r="J76" s="38"/>
-      <c r="K76" s="108" t="str">
+      <c r="K76" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT073</v>
       </c>
@@ -5304,7 +5436,7 @@
       <c r="H77" s="8"/>
       <c r="I77" s="38"/>
       <c r="J77" s="38"/>
-      <c r="K77" s="108" t="str">
+      <c r="K77" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT074</v>
       </c>
@@ -5331,7 +5463,7 @@
       <c r="H78" s="8"/>
       <c r="I78" s="38"/>
       <c r="J78" s="38"/>
-      <c r="K78" s="108" t="str">
+      <c r="K78" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT075</v>
       </c>
@@ -5358,7 +5490,7 @@
       <c r="H79" s="8"/>
       <c r="I79" s="38"/>
       <c r="J79" s="38"/>
-      <c r="K79" s="108" t="str">
+      <c r="K79" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT076</v>
       </c>
@@ -5385,7 +5517,7 @@
       <c r="H80" s="8"/>
       <c r="I80" s="38"/>
       <c r="J80" s="38"/>
-      <c r="K80" s="108" t="str">
+      <c r="K80" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT077</v>
       </c>
@@ -5412,7 +5544,7 @@
       <c r="H81" s="8"/>
       <c r="I81" s="38"/>
       <c r="J81" s="38"/>
-      <c r="K81" s="108" t="str">
+      <c r="K81" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT078</v>
       </c>
@@ -5439,7 +5571,7 @@
       <c r="H82" s="8"/>
       <c r="I82" s="38"/>
       <c r="J82" s="38"/>
-      <c r="K82" s="108" t="str">
+      <c r="K82" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT079</v>
       </c>
@@ -5466,7 +5598,7 @@
       <c r="H83" s="8"/>
       <c r="I83" s="38"/>
       <c r="J83" s="38"/>
-      <c r="K83" s="108" t="str">
+      <c r="K83" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT080</v>
       </c>
@@ -5493,7 +5625,7 @@
       <c r="H84" s="8"/>
       <c r="I84" s="38"/>
       <c r="J84" s="38"/>
-      <c r="K84" s="108" t="str">
+      <c r="K84" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT081</v>
       </c>
@@ -5520,7 +5652,7 @@
       <c r="H85" s="8"/>
       <c r="I85" s="38"/>
       <c r="J85" s="38"/>
-      <c r="K85" s="108" t="str">
+      <c r="K85" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT082</v>
       </c>
@@ -5547,7 +5679,7 @@
       <c r="H86" s="8"/>
       <c r="I86" s="38"/>
       <c r="J86" s="38"/>
-      <c r="K86" s="108" t="str">
+      <c r="K86" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT083</v>
       </c>
@@ -5574,7 +5706,7 @@
       <c r="H87" s="8"/>
       <c r="I87" s="38"/>
       <c r="J87" s="38"/>
-      <c r="K87" s="108" t="str">
+      <c r="K87" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT084</v>
       </c>
@@ -5601,7 +5733,7 @@
       <c r="H88" s="8"/>
       <c r="I88" s="38"/>
       <c r="J88" s="38"/>
-      <c r="K88" s="108" t="str">
+      <c r="K88" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT085</v>
       </c>
@@ -5628,7 +5760,7 @@
       <c r="H89" s="8"/>
       <c r="I89" s="38"/>
       <c r="J89" s="38"/>
-      <c r="K89" s="108" t="str">
+      <c r="K89" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT086</v>
       </c>
@@ -5655,7 +5787,7 @@
       <c r="H90" s="8"/>
       <c r="I90" s="38"/>
       <c r="J90" s="38"/>
-      <c r="K90" s="108" t="str">
+      <c r="K90" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT087</v>
       </c>
@@ -5682,7 +5814,7 @@
       <c r="H91" s="8"/>
       <c r="I91" s="38"/>
       <c r="J91" s="38"/>
-      <c r="K91" s="108" t="str">
+      <c r="K91" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT088</v>
       </c>
@@ -5709,7 +5841,7 @@
       <c r="H92" s="8"/>
       <c r="I92" s="38"/>
       <c r="J92" s="38"/>
-      <c r="K92" s="108" t="str">
+      <c r="K92" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT089</v>
       </c>
@@ -5736,7 +5868,7 @@
       <c r="H93" s="8"/>
       <c r="I93" s="38"/>
       <c r="J93" s="38"/>
-      <c r="K93" s="108" t="str">
+      <c r="K93" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT090</v>
       </c>
@@ -5763,7 +5895,7 @@
       <c r="H94" s="8"/>
       <c r="I94" s="38"/>
       <c r="J94" s="38"/>
-      <c r="K94" s="108" t="str">
+      <c r="K94" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT091</v>
       </c>
@@ -5790,7 +5922,7 @@
       <c r="H95" s="8"/>
       <c r="I95" s="38"/>
       <c r="J95" s="38"/>
-      <c r="K95" s="108" t="str">
+      <c r="K95" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT092</v>
       </c>
@@ -5817,7 +5949,7 @@
       <c r="H96" s="8"/>
       <c r="I96" s="38"/>
       <c r="J96" s="38"/>
-      <c r="K96" s="108" t="str">
+      <c r="K96" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT093</v>
       </c>
@@ -5844,7 +5976,7 @@
       <c r="H97" s="8"/>
       <c r="I97" s="38"/>
       <c r="J97" s="38"/>
-      <c r="K97" s="108" t="str">
+      <c r="K97" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT094</v>
       </c>
@@ -5871,7 +6003,7 @@
       <c r="H98" s="8"/>
       <c r="I98" s="38"/>
       <c r="J98" s="38"/>
-      <c r="K98" s="108" t="str">
+      <c r="K98" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT095</v>
       </c>
@@ -5898,7 +6030,7 @@
       <c r="H99" s="8"/>
       <c r="I99" s="38"/>
       <c r="J99" s="38"/>
-      <c r="K99" s="108" t="str">
+      <c r="K99" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT096</v>
       </c>
@@ -5925,7 +6057,7 @@
       <c r="H100" s="8"/>
       <c r="I100" s="38"/>
       <c r="J100" s="38"/>
-      <c r="K100" s="108" t="str">
+      <c r="K100" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT097</v>
       </c>
@@ -5952,7 +6084,7 @@
       <c r="H101" s="8"/>
       <c r="I101" s="38"/>
       <c r="J101" s="38"/>
-      <c r="K101" s="108" t="str">
+      <c r="K101" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT098</v>
       </c>
@@ -5979,7 +6111,7 @@
       <c r="H102" s="8"/>
       <c r="I102" s="38"/>
       <c r="J102" s="38"/>
-      <c r="K102" s="108" t="str">
+      <c r="K102" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT099</v>
       </c>
@@ -6006,7 +6138,7 @@
       <c r="H103" s="8"/>
       <c r="I103" s="38"/>
       <c r="J103" s="38"/>
-      <c r="K103" s="108" t="str">
+      <c r="K103" s="66" t="str">
         <f t="shared" si="9"/>
         <v>OPARTGT100</v>
       </c>
@@ -8179,65 +8311,65 @@
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="49.9" customHeight="1">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:11" ht="49.95" customHeight="1">
+      <c r="A1" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="66"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A2" s="67" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="96"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1">
+      <c r="A2" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="68"/>
+      <c r="B2" s="98"/>
       <c r="C2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="70"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="100"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1">
       <c r="K3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75">
-      <c r="A4" s="74" t="s">
+    <row r="4" spans="1:11" ht="15.6">
+      <c r="A4" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="76"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="106"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="33" t="s">
@@ -8359,7 +8491,7 @@
       <c r="H12" s="24"/>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1">
+    <row r="13" spans="1:11" ht="15" thickBot="1">
       <c r="A13" s="26">
         <v>8</v>
       </c>
@@ -8372,7 +8504,7 @@
       <c r="H13" s="27"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+    <row r="14" spans="1:11" ht="15" thickBot="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -8383,18 +8515,18 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="77" t="s">
+    <row r="15" spans="1:11" ht="15.6">
+      <c r="A15" s="87" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="89"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="20" t="s">
@@ -8409,15 +8541,15 @@
       <c r="D16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="82" t="s">
+      <c r="E16" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="87"/>
-      <c r="G16" s="82" t="s">
+      <c r="F16" s="93"/>
+      <c r="G16" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="83"/>
-      <c r="I16" s="84"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="92"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="21">
@@ -8426,11 +8558,11 @@
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="85"/>
-      <c r="I17" s="86"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="85"/>
       <c r="K17" t="s">
         <v>67</v>
       </c>
@@ -8442,11 +8574,11 @@
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="81"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="85"/>
-      <c r="I18" s="86"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="85"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="21">
@@ -8455,11 +8587,11 @@
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="86"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="85"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="21">
@@ -8468,11 +8600,11 @@
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="86"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="85"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="21">
@@ -8481,11 +8613,11 @@
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="86"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="85"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="21">
@@ -8494,11 +8626,11 @@
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="85"/>
-      <c r="I22" s="86"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="85"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="21">
@@ -8507,11 +8639,11 @@
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="86"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="85"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="21">
@@ -8520,11 +8652,11 @@
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="85"/>
-      <c r="I24" s="86"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="85"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="21">
@@ -8533,36 +8665,32 @@
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="91"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1">
+      <c r="E25" s="75"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="78"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="22">
         <v>10</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="94"/>
-      <c r="I26" s="95"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A4:I4"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
@@ -8577,11 +8705,15 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8597,63 +8729,63 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="49.9" customHeight="1">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:17" ht="49.95" customHeight="1">
+      <c r="A1" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="66"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="67" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="96"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" thickBot="1">
+      <c r="A2" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="68"/>
+      <c r="B2" s="98"/>
       <c r="C2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="69" t="s">
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="70"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1"/>
-    <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="74" t="s">
+      <c r="I2" s="100"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" thickBot="1"/>
+    <row r="4" spans="1:17" ht="15.6">
+      <c r="A4" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="76"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="106"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="33" t="s">
@@ -8687,7 +8819,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="34.5">
+    <row r="6" spans="1:17" ht="31.8">
       <c r="A6" s="23">
         <v>1</v>
       </c>
@@ -8715,15 +8847,15 @@
       <c r="I6" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="100" t="s">
+      <c r="K6" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="100"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="100"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="107"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="107"/>
+      <c r="Q6" s="107"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="23">
@@ -8753,15 +8885,15 @@
       <c r="I7" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="K7" s="100" t="s">
+      <c r="K7" s="107" t="s">
         <v>117</v>
       </c>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100"/>
-      <c r="Q7" s="100"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="107"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="23">
@@ -8844,7 +8976,7 @@
       <c r="H12" s="24"/>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1">
+    <row r="13" spans="1:17" ht="15" thickBot="1">
       <c r="A13" s="26">
         <v>8</v>
       </c>
@@ -8857,7 +8989,7 @@
       <c r="H13" s="27"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1">
+    <row r="14" spans="1:17" ht="15" thickBot="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -8868,18 +9000,18 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="77" t="s">
+    <row r="15" spans="1:17" ht="15.6">
+      <c r="A15" s="87" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="89"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="20" t="s">
@@ -8894,15 +9026,15 @@
       <c r="D16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="82" t="s">
+      <c r="E16" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="87"/>
-      <c r="G16" s="82" t="s">
+      <c r="F16" s="93"/>
+      <c r="G16" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="83"/>
-      <c r="I16" s="84"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="92"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="21">
@@ -8917,17 +9049,17 @@
       <c r="D17" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="96" t="s">
+      <c r="E17" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="97"/>
-      <c r="G17" s="96" t="s">
+      <c r="F17" s="109"/>
+      <c r="G17" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="98"/>
-      <c r="I17" s="99"/>
-    </row>
-    <row r="18" spans="1:11" ht="23.25">
+      <c r="H17" s="110"/>
+      <c r="I17" s="111"/>
+    </row>
+    <row r="18" spans="1:11" ht="21.6">
       <c r="A18" s="21">
         <v>2</v>
       </c>
@@ -8940,17 +9072,17 @@
       <c r="D18" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="96" t="s">
+      <c r="E18" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="97"/>
-      <c r="G18" s="96" t="s">
+      <c r="F18" s="109"/>
+      <c r="G18" s="108" t="s">
         <v>96</v>
       </c>
-      <c r="H18" s="98"/>
-      <c r="I18" s="99"/>
-    </row>
-    <row r="19" spans="1:11" ht="34.5">
+      <c r="H18" s="110"/>
+      <c r="I18" s="111"/>
+    </row>
+    <row r="19" spans="1:11" ht="31.8">
       <c r="A19" s="21">
         <v>3</v>
       </c>
@@ -8963,15 +9095,15 @@
       <c r="D19" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="96" t="s">
+      <c r="E19" s="108" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="97"/>
-      <c r="G19" s="96" t="s">
+      <c r="F19" s="109"/>
+      <c r="G19" s="108" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="98"/>
-      <c r="I19" s="99"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="111"/>
       <c r="K19" t="s">
         <v>67</v>
       </c>
@@ -8983,11 +9115,11 @@
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="86"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="85"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="21">
@@ -8996,11 +9128,11 @@
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="86"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="85"/>
       <c r="K21" t="s">
         <v>92</v>
       </c>
@@ -9012,11 +9144,11 @@
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="85"/>
-      <c r="I22" s="86"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="85"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="21">
@@ -9025,11 +9157,11 @@
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="86"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="85"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="21">
@@ -9038,11 +9170,11 @@
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="85"/>
-      <c r="I24" s="86"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="85"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="21">
@@ -9051,27 +9183,41 @@
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="91"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1">
+      <c r="E25" s="75"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="78"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="22">
         <v>10</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="94"/>
-      <c r="I26" s="95"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="K6:Q6"/>
@@ -9088,20 +9234,6 @@
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:I20"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9117,18 +9249,18 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:3">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="112" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="102"/>
-      <c r="C5" s="102"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="35" t="s">
@@ -9141,7 +9273,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="28.8">
       <c r="A7" s="37" t="s">
         <v>87</v>
       </c>
@@ -9152,11 +9284,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="60">
+    <row r="8" spans="1:3" ht="57.6">
       <c r="A8" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="112" t="s">
+      <c r="B8" s="69" t="s">
         <v>258</v>
       </c>
       <c r="C8" s="36" t="s">
@@ -9174,7 +9306,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45">
+    <row r="10" spans="1:3" ht="43.2">
       <c r="A10" s="37" t="s">
         <v>100</v>
       </c>
@@ -9197,131 +9329,222 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C28"/>
+  <dimension ref="B2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75">
-      <c r="B2" s="111" t="s">
+    <row r="2" spans="2:6" ht="15.6">
+      <c r="B2" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="111"/>
-    </row>
-    <row r="3" spans="2:3" ht="15" customHeight="1">
-      <c r="B3" s="114" t="s">
+      <c r="C2" s="113"/>
+    </row>
+    <row r="3" spans="2:6" ht="15" customHeight="1">
+      <c r="B3" s="71" t="s">
         <v>262</v>
       </c>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="70" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-    </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="38"/>
+    <row r="4" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B4" s="115">
+        <v>1</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="115">
+        <v>2</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="115">
+        <v>3</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="115">
+        <v>4</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="115">
+        <v>5</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="115">
+        <v>6</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="115">
+        <v>7</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="115">
+        <v>8</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="115">
+        <v>9</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="D12" t="s">
+        <v>281</v>
+      </c>
+      <c r="E12" t="s">
+        <v>282</v>
+      </c>
+      <c r="F12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B13" s="115">
+        <v>10</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="D13" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="115">
+        <v>11</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="115">
+        <v>12</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="115">
+        <v>13</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="115">
+        <v>14</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="115">
+        <v>15</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>287</v>
+      </c>
+      <c r="D18" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="115">
+        <v>16</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="115"/>
       <c r="C20" s="38"/>
     </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="38"/>
+    <row r="21" spans="2:4">
+      <c r="B21" s="115"/>
       <c r="C21" s="38"/>
     </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="38"/>
+    <row r="22" spans="2:4">
+      <c r="B22" s="115"/>
       <c r="C22" s="38"/>
     </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="38"/>
+    <row r="23" spans="2:4">
+      <c r="B23" s="115"/>
       <c r="C23" s="38"/>
     </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="38"/>
+    <row r="24" spans="2:4">
+      <c r="B24" s="115"/>
       <c r="C24" s="38"/>
     </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="38"/>
+    <row r="25" spans="2:4">
+      <c r="B25" s="115"/>
       <c r="C25" s="38"/>
     </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="38"/>
+    <row r="26" spans="2:4">
+      <c r="B26" s="115"/>
       <c r="C26" s="38"/>
     </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="38"/>
+    <row r="27" spans="2:4">
+      <c r="B27" s="115"/>
       <c r="C27" s="38"/>
     </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="38"/>
+    <row r="28" spans="2:4">
+      <c r="B28" s="115"/>
       <c r="C28" s="38"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="116"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" t="s">
+        <v>267</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9340,63 +9563,63 @@
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" ht="15.75">
-      <c r="A3" s="111" t="s">
+    <row r="3" spans="1:3" ht="15.6">
+      <c r="A3" s="113" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="112" t="s">
         <v>260</v>
       </c>
-      <c r="C4" s="102"/>
+      <c r="C4" s="112"/>
     </row>
     <row r="5" spans="1:3" ht="96" customHeight="1">
       <c r="A5" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="114" t="s">
         <v>259</v>
       </c>
-      <c r="C5" s="101"/>
+      <c r="C5" s="114"/>
     </row>
     <row r="6" spans="1:3" ht="64.5" customHeight="1">
       <c r="A6" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="114" t="s">
         <v>254</v>
       </c>
-      <c r="C6" s="101"/>
+      <c r="C6" s="114"/>
     </row>
     <row r="7" spans="1:3" ht="67.5" customHeight="1">
       <c r="A7" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="114" t="s">
         <v>255</v>
       </c>
-      <c r="C7" s="101"/>
+      <c r="C7" s="114"/>
     </row>
     <row r="8" spans="1:3" ht="72.75" customHeight="1">
       <c r="A8" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="114" t="s">
         <v>261</v>
       </c>
-      <c r="C8" s="101"/>
+      <c r="C8" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -9420,23 +9643,23 @@
       <selection activeCell="C14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75">
-      <c r="B2" s="111" t="s">
+    <row r="2" spans="2:3" ht="15.6">
+      <c r="B2" s="113" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="111"/>
+      <c r="C2" s="113"/>
     </row>
     <row r="3" spans="2:3" ht="15" customHeight="1">
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="70" t="s">
         <v>264</v>
       </c>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="70" t="s">
         <v>107</v>
       </c>
     </row>
@@ -9490,9 +9713,9 @@
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
@@ -9508,7 +9731,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="7.15" customHeight="1"/>
+    <row r="4" spans="2:3" ht="7.2" customHeight="1"/>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>53</v>

</xml_diff>